<commit_message>
Jata Input edits 15/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
@@ -4630,7 +4630,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="64">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4774,9 +4774,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -5096,10 +5093,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1805" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="X1811" sqref="X1811"/>
+      <selection pane="bottomLeft" activeCell="X1448" sqref="X1448"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5594,49 +5591,49 @@
       <c r="I1" s="45" t="s">
         <v>181</v>
       </c>
-      <c r="J1" s="51" t="s">
+      <c r="J1" s="50" t="s">
         <v>182</v>
       </c>
-      <c r="K1" s="51" t="s">
+      <c r="K1" s="50" t="s">
         <v>13</v>
       </c>
-      <c r="L1" s="51" t="s">
+      <c r="L1" s="50" t="s">
         <v>11</v>
       </c>
-      <c r="M1" s="51" t="s">
+      <c r="M1" s="50" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="54" t="s">
+      <c r="N1" s="53" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="53" t="s">
+      <c r="O1" s="52" t="s">
         <v>2</v>
       </c>
-      <c r="P1" s="52" t="s">
+      <c r="P1" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="Q1" s="52" t="s">
+      <c r="Q1" s="51" t="s">
         <v>9</v>
       </c>
-      <c r="R1" s="52" t="s">
+      <c r="R1" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="51" t="s">
+      <c r="S1" s="50" t="s">
         <v>186</v>
       </c>
-      <c r="T1" s="51" t="s">
+      <c r="T1" s="50" t="s">
         <v>187</v>
       </c>
-      <c r="U1" s="51" t="s">
+      <c r="U1" s="50" t="s">
         <v>188</v>
       </c>
-      <c r="V1" s="51" t="s">
+      <c r="V1" s="50" t="s">
         <v>189</v>
       </c>
-      <c r="W1" s="51" t="s">
+      <c r="W1" s="50" t="s">
         <v>190</v>
       </c>
-      <c r="X1" s="52" t="s">
+      <c r="X1" s="51" t="s">
         <v>4</v>
       </c>
     </row>
@@ -5664,7 +5661,7 @@
       <c r="M2" s="5">
         <v>1</v>
       </c>
-      <c r="N2" s="55" t="s">
+      <c r="N2" s="54" t="s">
         <v>1056</v>
       </c>
       <c r="O2" s="7" t="s">
@@ -15793,7 +15790,7 @@
       <c r="F257" s="19"/>
       <c r="G257" s="19"/>
       <c r="H257" s="39"/>
-      <c r="I257" s="56" t="s">
+      <c r="I257" s="55" t="s">
         <v>1047</v>
       </c>
       <c r="J257" s="46">
@@ -15811,7 +15808,7 @@
         <f t="shared" si="10"/>
         <v>43</v>
       </c>
-      <c r="N257" s="57" t="s">
+      <c r="N257" s="56" t="s">
         <v>719</v>
       </c>
       <c r="O257" s="33"/>
@@ -15825,7 +15822,7 @@
       <c r="U257" s="7"/>
       <c r="V257" s="7"/>
       <c r="W257" s="7"/>
-      <c r="X257" s="57" t="s">
+      <c r="X257" s="56" t="s">
         <v>1079</v>
       </c>
     </row>
@@ -20045,7 +20042,7 @@
       <c r="F365" s="19"/>
       <c r="G365" s="19"/>
       <c r="H365" s="39"/>
-      <c r="I365" s="56" t="s">
+      <c r="I365" s="55" t="s">
         <v>1042</v>
       </c>
       <c r="J365" s="46">
@@ -20063,7 +20060,7 @@
         <f t="shared" si="12"/>
         <v>26</v>
       </c>
-      <c r="N365" s="57" t="s">
+      <c r="N365" s="56" t="s">
         <v>22</v>
       </c>
       <c r="O365" s="33"/>
@@ -20077,7 +20074,7 @@
       <c r="U365" s="7"/>
       <c r="V365" s="7"/>
       <c r="W365" s="7"/>
-      <c r="X365" s="57" t="s">
+      <c r="X365" s="56" t="s">
         <v>1132</v>
       </c>
     </row>
@@ -21703,7 +21700,7 @@
       <c r="F408" s="19"/>
       <c r="G408" s="19"/>
       <c r="H408" s="19"/>
-      <c r="I408" s="56" t="s">
+      <c r="I408" s="55" t="s">
         <v>1041</v>
       </c>
       <c r="J408" s="46">
@@ -21721,7 +21718,7 @@
         <f t="shared" si="14"/>
         <v>43</v>
       </c>
-      <c r="N408" s="57" t="s">
+      <c r="N408" s="56" t="s">
         <v>651</v>
       </c>
       <c r="O408" s="33"/>
@@ -21735,7 +21732,7 @@
       <c r="U408" s="7"/>
       <c r="V408" s="7"/>
       <c r="W408" s="7"/>
-      <c r="X408" s="57" t="s">
+      <c r="X408" s="56" t="s">
         <v>1140</v>
       </c>
     </row>
@@ -33072,7 +33069,7 @@
       <c r="F700" s="19"/>
       <c r="G700" s="19"/>
       <c r="H700" s="19"/>
-      <c r="I700" s="56" t="s">
+      <c r="I700" s="55" t="s">
         <v>1030</v>
       </c>
       <c r="J700" s="46">
@@ -33090,7 +33087,7 @@
         <f t="shared" si="24"/>
         <v>20</v>
       </c>
-      <c r="N700" s="57" t="s">
+      <c r="N700" s="56" t="s">
         <v>1175</v>
       </c>
       <c r="O700" s="33" t="s">
@@ -33104,7 +33101,7 @@
       <c r="U700" s="7"/>
       <c r="V700" s="7"/>
       <c r="W700" s="7"/>
-      <c r="X700" s="57" t="s">
+      <c r="X700" s="56" t="s">
         <v>728</v>
       </c>
     </row>
@@ -33279,7 +33276,7 @@
         <f t="shared" si="24"/>
         <v>25</v>
       </c>
-      <c r="N705" s="57" t="s">
+      <c r="N705" s="56" t="s">
         <v>1175</v>
       </c>
       <c r="O705" s="6" t="s">
@@ -33302,7 +33299,7 @@
       <c r="F706" s="19"/>
       <c r="G706" s="19"/>
       <c r="H706" s="19"/>
-      <c r="I706" s="56" t="s">
+      <c r="I706" s="55" t="s">
         <v>1030</v>
       </c>
       <c r="J706" s="46">
@@ -33320,7 +33317,7 @@
         <f t="shared" si="24"/>
         <v>26</v>
       </c>
-      <c r="N706" s="57" t="s">
+      <c r="N706" s="56" t="s">
         <v>719</v>
       </c>
       <c r="O706" s="7"/>
@@ -33334,7 +33331,7 @@
       <c r="U706" s="7"/>
       <c r="V706" s="7"/>
       <c r="W706" s="7"/>
-      <c r="X706" s="57" t="s">
+      <c r="X706" s="56" t="s">
         <v>1079</v>
       </c>
     </row>
@@ -36223,7 +36220,7 @@
       <c r="F783" s="19"/>
       <c r="G783" s="19"/>
       <c r="H783" s="19"/>
-      <c r="I783" s="56" t="s">
+      <c r="I783" s="55" t="s">
         <v>1029</v>
       </c>
       <c r="J783" s="46">
@@ -36241,7 +36238,7 @@
         <f t="shared" si="26"/>
         <v>77</v>
       </c>
-      <c r="N783" s="57" t="s">
+      <c r="N783" s="56" t="s">
         <v>688</v>
       </c>
       <c r="O783" s="7"/>
@@ -36255,7 +36252,7 @@
       <c r="U783" s="7"/>
       <c r="V783" s="7"/>
       <c r="W783" s="7"/>
-      <c r="X783" s="57" t="s">
+      <c r="X783" s="56" t="s">
         <v>1191</v>
       </c>
     </row>
@@ -36361,10 +36358,10 @@
       <c r="P786" s="7"/>
       <c r="Q786" s="7"/>
       <c r="R786" s="7"/>
-      <c r="S786" s="62" t="s">
+      <c r="S786" s="61" t="s">
         <v>1439</v>
       </c>
-      <c r="T786" s="62" t="s">
+      <c r="T786" s="61" t="s">
         <v>1442</v>
       </c>
       <c r="U786" s="7"/>
@@ -39171,7 +39168,7 @@
       <c r="U859" s="7"/>
       <c r="V859" s="7"/>
       <c r="W859" s="7"/>
-      <c r="X859" s="57" t="s">
+      <c r="X859" s="56" t="s">
         <v>1459</v>
       </c>
     </row>
@@ -44828,7 +44825,7 @@
       <c r="F1008" s="19"/>
       <c r="G1008" s="19"/>
       <c r="H1008" s="19"/>
-      <c r="I1008" s="56" t="s">
+      <c r="I1008" s="55" t="s">
         <v>1017</v>
       </c>
       <c r="J1008" s="46">
@@ -44846,7 +44843,7 @@
         <f t="shared" si="34"/>
         <v>19</v>
       </c>
-      <c r="N1008" s="57" t="s">
+      <c r="N1008" s="56" t="s">
         <v>580</v>
       </c>
       <c r="O1008" s="33"/>
@@ -44858,7 +44855,7 @@
       <c r="U1008" s="7"/>
       <c r="V1008" s="7"/>
       <c r="W1008" s="7"/>
-      <c r="X1008" s="57"/>
+      <c r="X1008" s="56"/>
     </row>
     <row r="1009" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1009" s="19"/>
@@ -47479,7 +47476,7 @@
         <f t="shared" si="36"/>
         <v>10</v>
       </c>
-      <c r="N1077" s="57" t="s">
+      <c r="N1077" s="56" t="s">
         <v>1261</v>
       </c>
       <c r="O1077" s="6" t="s">
@@ -53858,7 +53855,7 @@
         <f t="shared" si="40"/>
         <v>20</v>
       </c>
-      <c r="N1245" s="57" t="s">
+      <c r="N1245" s="56" t="s">
         <v>1056</v>
       </c>
       <c r="O1245" s="6" t="s">
@@ -53872,7 +53869,7 @@
       <c r="U1245" s="7"/>
       <c r="V1245" s="7"/>
       <c r="W1245" s="7"/>
-      <c r="X1245" s="57"/>
+      <c r="X1245" s="56"/>
     </row>
     <row r="1246" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1246" s="19"/>
@@ -57602,10 +57599,10 @@
         <f t="shared" si="44"/>
         <v>118</v>
       </c>
-      <c r="N1343" s="57" t="s">
+      <c r="N1343" s="56" t="s">
         <v>441</v>
       </c>
-      <c r="O1343" s="60" t="s">
+      <c r="O1343" s="59" t="s">
         <v>1064</v>
       </c>
       <c r="P1343" s="7" t="s">
@@ -57618,7 +57615,7 @@
       <c r="U1343" s="7"/>
       <c r="V1343" s="7"/>
       <c r="W1343" s="7"/>
-      <c r="X1343" s="59" t="s">
+      <c r="X1343" s="58" t="s">
         <v>1463</v>
       </c>
     </row>
@@ -59876,7 +59873,7 @@
         <f t="shared" si="46"/>
         <v>59</v>
       </c>
-      <c r="N1402" s="57" t="s">
+      <c r="N1402" s="56" t="s">
         <v>1314</v>
       </c>
       <c r="O1402" s="6"/>
@@ -61643,7 +61640,7 @@
       <c r="U1448" s="7"/>
       <c r="V1448" s="7"/>
       <c r="W1448" s="7"/>
-      <c r="X1448" s="50" t="s">
+      <c r="X1448" s="56" t="s">
         <v>1474</v>
       </c>
     </row>
@@ -63238,7 +63235,7 @@
       <c r="F1491" s="19"/>
       <c r="G1491" s="19"/>
       <c r="H1491" s="19"/>
-      <c r="I1491" s="56" t="s">
+      <c r="I1491" s="55" t="s">
         <v>1004</v>
       </c>
       <c r="J1491" s="46">
@@ -63256,7 +63253,7 @@
         <f t="shared" si="48"/>
         <v>148</v>
       </c>
-      <c r="N1491" s="57" t="s">
+      <c r="N1491" s="56" t="s">
         <v>184</v>
       </c>
       <c r="O1491" s="33"/>
@@ -63270,7 +63267,7 @@
       <c r="U1491" s="7"/>
       <c r="V1491" s="7"/>
       <c r="W1491" s="7"/>
-      <c r="X1491" s="57" t="s">
+      <c r="X1491" s="56" t="s">
         <v>1328</v>
       </c>
     </row>
@@ -63595,7 +63592,7 @@
         <f t="shared" si="48"/>
         <v>9</v>
       </c>
-      <c r="N1500" s="50" t="s">
+      <c r="N1500" s="56" t="s">
         <v>371</v>
       </c>
       <c r="O1500" s="6"/>
@@ -63609,7 +63606,7 @@
       <c r="U1500" s="7"/>
       <c r="V1500" s="7"/>
       <c r="W1500" s="7"/>
-      <c r="X1500" s="50" t="s">
+      <c r="X1500" s="56" t="s">
         <v>1465</v>
       </c>
     </row>
@@ -67983,7 +67980,7 @@
         <f t="shared" si="52"/>
         <v>141</v>
       </c>
-      <c r="N1632" s="63" t="s">
+      <c r="N1632" s="62" t="s">
         <v>288</v>
       </c>
       <c r="X1632" s="43"/>
@@ -69234,13 +69231,13 @@
         <f t="shared" si="54"/>
         <v>33</v>
       </c>
-      <c r="N1680" s="57" t="s">
+      <c r="N1680" s="56" t="s">
         <v>273</v>
       </c>
       <c r="P1680" s="7" t="s">
         <v>1074</v>
       </c>
-      <c r="X1680" s="57" t="s">
+      <c r="X1680" s="56" t="s">
         <v>1469</v>
       </c>
     </row>
@@ -69292,7 +69289,7 @@
         <f t="shared" si="54"/>
         <v>35</v>
       </c>
-      <c r="N1682" s="57" t="s">
+      <c r="N1682" s="56" t="s">
         <v>1261</v>
       </c>
       <c r="X1682" s="43"/>
@@ -69924,7 +69921,7 @@
       <c r="X1706" s="43"/>
     </row>
     <row r="1707" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="I1707" s="56" t="s">
+      <c r="I1707" s="55" t="s">
         <v>999</v>
       </c>
       <c r="J1707" s="46">
@@ -69942,15 +69939,15 @@
         <f t="shared" si="54"/>
         <v>60</v>
       </c>
-      <c r="N1707" s="57" t="s">
+      <c r="N1707" s="56" t="s">
         <v>254</v>
       </c>
-      <c r="O1707" s="58"/>
+      <c r="O1707" s="57"/>
       <c r="P1707" s="7" t="s">
         <v>1074</v>
       </c>
       <c r="U1707" s="7"/>
-      <c r="X1707" s="57" t="s">
+      <c r="X1707" s="56" t="s">
         <v>1380</v>
       </c>
     </row>
@@ -72317,7 +72314,7 @@
       <c r="N1797" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="U1797" s="61" t="s">
+      <c r="U1797" s="60" t="s">
         <v>1451</v>
       </c>
       <c r="X1797" s="43"/>
@@ -72344,7 +72341,7 @@
       <c r="N1798" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="U1798" s="61" t="s">
+      <c r="U1798" s="60" t="s">
         <v>1441</v>
       </c>
       <c r="X1798" s="43"/>

</xml_diff>

<commit_message>
Padam input corrections Trikramam table 16/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4735" uniqueCount="1477">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="1481">
   <si>
     <t>Passage</t>
   </si>
@@ -4295,9 +4295,6 @@
     <t>uqBe ityuqBe |</t>
   </si>
   <si>
-    <t>janma#nIq ||</t>
-  </si>
-  <si>
     <t>vaqriqvoqvitta#rA |</t>
   </si>
   <si>
@@ -4361,9 +4358,6 @@
     <t>vis</t>
   </si>
   <si>
-    <t>se?re?</t>
-  </si>
-  <si>
     <t>EL</t>
   </si>
   <si>
@@ -4421,9 +4415,6 @@
     <t>saq(gg)qskRuqtamiti# sa(gg)skRuqtam ||</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>uqvityu# ||</t>
   </si>
   <si>
@@ -4458,6 +4449,27 @@
   </si>
   <si>
     <t>jyotiqShetiq jyoti#ShA ||</t>
+  </si>
+  <si>
+    <t>janma#nI ||</t>
+  </si>
+  <si>
+    <t>RE?</t>
+  </si>
+  <si>
+    <t>ShoqDaqSinaq iti# ShoDaqSine$ ||</t>
+  </si>
+  <si>
+    <t>NE+NRE</t>
+  </si>
+  <si>
+    <t>NE+NSE+??</t>
+  </si>
+  <si>
+    <t>se?</t>
+  </si>
+  <si>
+    <t>NRE+se?</t>
   </si>
 </sst>
 </file>
@@ -4583,7 +4595,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4599,6 +4611,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4630,7 +4648,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="73">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4805,11 +4823,39 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5093,10 +5139,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1802" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="X1448" sqref="X1448"/>
+      <selection pane="bottomLeft" activeCell="U1798" sqref="U1798"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5111,14 +5157,15 @@
     <col min="10" max="10" width="12.85546875" style="46" customWidth="1"/>
     <col min="11" max="11" width="13.5703125" style="17" customWidth="1"/>
     <col min="12" max="12" width="15.5703125" style="17" customWidth="1"/>
-    <col min="13" max="13" width="16.28515625" style="5" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" style="5" customWidth="1"/>
     <col min="14" max="14" width="39.85546875" style="4" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="10" style="3" customWidth="1"/>
     <col min="16" max="17" width="5.7109375" style="1" customWidth="1"/>
     <col min="18" max="18" width="6.28515625" style="1" customWidth="1"/>
     <col min="19" max="19" width="12.42578125" style="1" customWidth="1"/>
     <col min="20" max="20" width="10" style="1" customWidth="1"/>
-    <col min="21" max="22" width="18.5703125" style="1" customWidth="1"/>
+    <col min="21" max="21" width="18.5703125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="15.85546875" style="1" customWidth="1"/>
     <col min="23" max="23" width="11.7109375" style="1" hidden="1" customWidth="1"/>
     <col min="24" max="24" width="89.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="25" max="265" width="9.140625" style="2"/>
@@ -5839,7 +5886,7 @@
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="11" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
@@ -8618,7 +8665,7 @@
       <c r="V73" s="11"/>
       <c r="W73" s="11"/>
       <c r="X73" s="43" t="s">
-        <v>1457</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="74" spans="1:24" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -9629,7 +9676,7 @@
       <c r="Q99" s="7"/>
       <c r="R99" s="7"/>
       <c r="S99" s="7" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="T99" s="7"/>
       <c r="U99" s="7"/>
@@ -10091,10 +10138,10 @@
       <c r="Q111" s="7"/>
       <c r="R111" s="7"/>
       <c r="S111" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="T111" s="7" t="s">
         <v>1439</v>
-      </c>
-      <c r="T111" s="7" t="s">
-        <v>1440</v>
       </c>
       <c r="U111" s="7"/>
       <c r="V111" s="7"/>
@@ -10327,7 +10374,7 @@
       <c r="S117" s="7"/>
       <c r="T117" s="7"/>
       <c r="U117" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V117" s="7"/>
       <c r="W117" s="7"/>
@@ -10907,10 +10954,10 @@
       <c r="Q132" s="7"/>
       <c r="R132" s="7"/>
       <c r="S132" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="T132" s="7" t="s">
         <v>1439</v>
-      </c>
-      <c r="T132" s="7" t="s">
-        <v>1440</v>
       </c>
       <c r="U132" s="7"/>
       <c r="V132" s="7"/>
@@ -10987,10 +11034,10 @@
       <c r="Q134" s="7"/>
       <c r="R134" s="7"/>
       <c r="S134" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="T134" s="7" t="s">
         <v>1439</v>
-      </c>
-      <c r="T134" s="7" t="s">
-        <v>1440</v>
       </c>
       <c r="U134" s="7"/>
       <c r="V134" s="7"/>
@@ -11998,10 +12045,10 @@
       <c r="Q160" s="7"/>
       <c r="R160" s="7"/>
       <c r="S160" s="7" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="T160" s="7" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="U160" s="7"/>
       <c r="V160" s="7"/>
@@ -12388,10 +12435,10 @@
       <c r="Q170" s="7"/>
       <c r="R170" s="7"/>
       <c r="S170" s="7" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="T170" s="7" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="U170" s="7"/>
       <c r="V170" s="7"/>
@@ -12548,10 +12595,10 @@
       <c r="Q174" s="7"/>
       <c r="R174" s="7"/>
       <c r="S174" s="7" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="T174" s="7" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="U174" s="7"/>
       <c r="V174" s="7"/>
@@ -13138,10 +13185,10 @@
       <c r="Q189" s="7"/>
       <c r="R189" s="7"/>
       <c r="S189" s="7" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="T189" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="U189" s="7"/>
       <c r="V189" s="7"/>
@@ -13218,10 +13265,10 @@
       <c r="Q191" s="7"/>
       <c r="R191" s="7"/>
       <c r="S191" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="T191" s="7" t="s">
         <v>1439</v>
-      </c>
-      <c r="T191" s="7" t="s">
-        <v>1440</v>
       </c>
       <c r="U191" s="7"/>
       <c r="V191" s="7"/>
@@ -14634,7 +14681,7 @@
       <c r="S227" s="7"/>
       <c r="T227" s="7"/>
       <c r="U227" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V227" s="7"/>
       <c r="W227" s="7"/>
@@ -17084,7 +17131,7 @@
       <c r="S289" s="7"/>
       <c r="T289" s="7"/>
       <c r="U289" s="37" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V289" s="7"/>
       <c r="W289" s="7"/>
@@ -17834,7 +17881,7 @@
       <c r="S308" s="7"/>
       <c r="T308" s="7"/>
       <c r="U308" s="37" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V308" s="7"/>
       <c r="W308" s="7"/>
@@ -18030,7 +18077,7 @@
       <c r="S313" s="7"/>
       <c r="T313" s="7"/>
       <c r="U313" s="37" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V313" s="7"/>
       <c r="W313" s="7"/>
@@ -21156,7 +21203,7 @@
       <c r="S393" s="7"/>
       <c r="T393" s="7"/>
       <c r="U393" s="7" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V393" s="7"/>
       <c r="W393" s="7"/>
@@ -22192,7 +22239,7 @@
       <c r="S420" s="7"/>
       <c r="T420" s="7"/>
       <c r="U420" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V420" s="7"/>
       <c r="W420" s="7"/>
@@ -22784,7 +22831,7 @@
       <c r="S435" s="7"/>
       <c r="T435" s="7"/>
       <c r="U435" s="7" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V435" s="7"/>
       <c r="W435" s="7"/>
@@ -23328,13 +23375,13 @@
       <c r="F450" s="19"/>
       <c r="G450" s="19"/>
       <c r="H450" s="19"/>
-      <c r="I450" s="48" t="s">
+      <c r="I450" s="55" t="s">
         <v>1040</v>
       </c>
       <c r="J450" s="46">
         <v>12</v>
       </c>
-      <c r="K450" s="16">
+      <c r="K450" s="5">
         <f t="shared" si="15"/>
         <v>449</v>
       </c>
@@ -23346,7 +23393,7 @@
         <f t="shared" si="16"/>
         <v>42</v>
       </c>
-      <c r="N450" s="43" t="s">
+      <c r="N450" s="56" t="s">
         <v>651</v>
       </c>
       <c r="O450" s="7"/>
@@ -23360,7 +23407,7 @@
       <c r="U450" s="7"/>
       <c r="V450" s="7"/>
       <c r="W450" s="7"/>
-      <c r="X450" s="43" t="s">
+      <c r="X450" s="56" t="s">
         <v>1141</v>
       </c>
     </row>
@@ -24324,7 +24371,7 @@
       <c r="S475" s="7"/>
       <c r="T475" s="7"/>
       <c r="U475" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V475" s="7"/>
       <c r="W475" s="7"/>
@@ -29616,7 +29663,7 @@
       <c r="S611" s="7"/>
       <c r="T611" s="7"/>
       <c r="U611" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V611" s="7"/>
       <c r="W611" s="7"/>
@@ -30476,12 +30523,12 @@
       <c r="Q633" s="7"/>
       <c r="R633" s="7"/>
       <c r="S633" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T633" s="7"/>
       <c r="U633" s="7"/>
       <c r="V633" s="7" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="W633" s="7"/>
       <c r="X633" s="43"/>
@@ -30632,7 +30679,7 @@
       <c r="Q637" s="7"/>
       <c r="R637" s="7"/>
       <c r="S637" s="7" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="T637" s="7"/>
       <c r="U637" s="7"/>
@@ -31608,12 +31655,12 @@
       <c r="Q662" s="7"/>
       <c r="R662" s="7"/>
       <c r="S662" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T662" s="7"/>
       <c r="U662" s="7"/>
       <c r="V662" s="7" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="W662" s="7"/>
       <c r="X662" s="43"/>
@@ -31804,12 +31851,12 @@
       <c r="Q667" s="7"/>
       <c r="R667" s="7"/>
       <c r="S667" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T667" s="7"/>
       <c r="U667" s="7"/>
       <c r="V667" s="7" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="W667" s="7"/>
       <c r="X667" s="43" t="s">
@@ -32348,12 +32395,12 @@
       <c r="Q681" s="7"/>
       <c r="R681" s="7"/>
       <c r="S681" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T681" s="7"/>
       <c r="U681" s="7"/>
       <c r="V681" s="7" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="W681" s="7"/>
       <c r="X681" s="43"/>
@@ -33630,7 +33677,7 @@
       <c r="V714" s="7"/>
       <c r="W714" s="7"/>
       <c r="X714" s="43" t="s">
-        <v>1470</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="715" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -34499,7 +34546,7 @@
         <v>31</v>
       </c>
       <c r="N737" s="43" t="s">
-        <v>1422</v>
+        <v>1474</v>
       </c>
       <c r="O737" s="6" t="s">
         <v>1075</v>
@@ -35112,7 +35159,7 @@
       <c r="Q753" s="7"/>
       <c r="R753" s="7"/>
       <c r="S753" s="7" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="T753" s="7"/>
       <c r="U753" s="7"/>
@@ -35158,7 +35205,7 @@
       <c r="V754" s="7"/>
       <c r="W754" s="7"/>
       <c r="X754" s="43" t="s">
-        <v>1471</v>
+        <v>1468</v>
       </c>
     </row>
     <row r="755" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -35487,7 +35534,7 @@
         <v>57</v>
       </c>
       <c r="N763" s="43" t="s">
-        <v>1423</v>
+        <v>1422</v>
       </c>
       <c r="O763" s="6" t="s">
         <v>1064</v>
@@ -36358,11 +36405,11 @@
       <c r="P786" s="7"/>
       <c r="Q786" s="7"/>
       <c r="R786" s="7"/>
-      <c r="S786" s="61" t="s">
-        <v>1439</v>
-      </c>
-      <c r="T786" s="61" t="s">
-        <v>1442</v>
+      <c r="S786" s="7" t="s">
+        <v>1438</v>
+      </c>
+      <c r="T786" s="7" t="s">
+        <v>1441</v>
       </c>
       <c r="U786" s="7"/>
       <c r="V786" s="7"/>
@@ -37242,10 +37289,10 @@
       <c r="Q809" s="7"/>
       <c r="R809" s="7"/>
       <c r="S809" s="37" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="T809" s="37" t="s">
-        <v>1472</v>
+        <v>1469</v>
       </c>
       <c r="U809" s="7"/>
       <c r="V809" s="7"/>
@@ -37704,7 +37751,7 @@
       <c r="Q821" s="7"/>
       <c r="R821" s="7"/>
       <c r="S821" s="7" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="T821" s="7"/>
       <c r="U821" s="7"/>
@@ -37821,7 +37868,7 @@
       <c r="S824" s="7"/>
       <c r="T824" s="7"/>
       <c r="U824" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V824" s="7"/>
       <c r="W824" s="7"/>
@@ -39157,7 +39204,7 @@
         <v>3</v>
       </c>
       <c r="N859" s="43" t="s">
-        <v>1458</v>
+        <v>1456</v>
       </c>
       <c r="O859" s="6"/>
       <c r="P859" s="7"/>
@@ -39169,7 +39216,7 @@
       <c r="V859" s="7"/>
       <c r="W859" s="7"/>
       <c r="X859" s="56" t="s">
-        <v>1459</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="860" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -39352,7 +39399,7 @@
         <v>8</v>
       </c>
       <c r="N864" s="44" t="s">
-        <v>1424</v>
+        <v>1423</v>
       </c>
       <c r="O864" s="6"/>
       <c r="P864" s="7"/>
@@ -39922,7 +39969,7 @@
         <v>8</v>
       </c>
       <c r="N879" s="43" t="s">
-        <v>1425</v>
+        <v>1424</v>
       </c>
       <c r="O879" s="6"/>
       <c r="P879" s="7"/>
@@ -40267,7 +40314,7 @@
         <v>17</v>
       </c>
       <c r="N888" s="43" t="s">
-        <v>1426</v>
+        <v>1425</v>
       </c>
       <c r="O888" s="6" t="s">
         <v>1064</v>
@@ -41490,7 +41537,7 @@
       <c r="V920" s="7"/>
       <c r="W920" s="7"/>
       <c r="X920" s="43" t="s">
-        <v>1427</v>
+        <v>1426</v>
       </c>
     </row>
     <row r="921" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -41667,7 +41714,7 @@
         <v>5</v>
       </c>
       <c r="N925" s="43" t="s">
-        <v>1428</v>
+        <v>1427</v>
       </c>
       <c r="O925" s="7" t="s">
         <v>1075</v>
@@ -41681,7 +41728,7 @@
       <c r="V925" s="7"/>
       <c r="W925" s="7"/>
       <c r="X925" s="43" t="s">
-        <v>1429</v>
+        <v>1428</v>
       </c>
     </row>
     <row r="926" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -41719,7 +41766,7 @@
       <c r="S926" s="7"/>
       <c r="T926" s="7"/>
       <c r="U926" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V926" s="7"/>
       <c r="W926" s="7"/>
@@ -41825,7 +41872,7 @@
         <v>9</v>
       </c>
       <c r="N929" s="43" t="s">
-        <v>1448</v>
+        <v>1446</v>
       </c>
       <c r="O929" s="6" t="s">
         <v>1075</v>
@@ -43323,7 +43370,7 @@
       <c r="Q968" s="7"/>
       <c r="R968" s="7"/>
       <c r="S968" s="7" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="T968" s="7"/>
       <c r="U968" s="7"/>
@@ -43440,7 +43487,7 @@
       <c r="Q971" s="7"/>
       <c r="R971" s="7"/>
       <c r="S971" s="7" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="T971" s="7"/>
       <c r="U971" s="7"/>
@@ -43787,7 +43834,7 @@
       <c r="Q980" s="7"/>
       <c r="R980" s="7"/>
       <c r="S980" s="7" t="s">
-        <v>1445</v>
+        <v>1443</v>
       </c>
       <c r="T980" s="7"/>
       <c r="U980" s="7"/>
@@ -43905,7 +43952,9 @@
       <c r="R983" s="7"/>
       <c r="S983" s="7"/>
       <c r="T983" s="7"/>
-      <c r="U983" s="7"/>
+      <c r="U983" s="7" t="s">
+        <v>1454</v>
+      </c>
       <c r="V983" s="7"/>
       <c r="W983" s="7"/>
       <c r="X983" s="43"/>
@@ -43934,7 +43983,7 @@
         <v>14</v>
       </c>
       <c r="N984" s="44" t="s">
-        <v>1430</v>
+        <v>1429</v>
       </c>
       <c r="O984" s="6" t="s">
         <v>1075</v>
@@ -43948,7 +43997,7 @@
       <c r="V984" s="7"/>
       <c r="W984" s="7"/>
       <c r="X984" s="44" t="s">
-        <v>1460</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="985" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -44095,7 +44144,7 @@
       <c r="S988" s="7"/>
       <c r="T988" s="7"/>
       <c r="U988" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V988" s="7"/>
       <c r="W988" s="7"/>
@@ -47908,7 +47957,7 @@
       <c r="W1088" s="7"/>
       <c r="X1088" s="43"/>
     </row>
-    <row r="1089" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1089" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1089" s="19"/>
       <c r="F1089" s="19"/>
       <c r="G1089" s="19"/>
@@ -47945,7 +47994,7 @@
       <c r="W1089" s="7"/>
       <c r="X1089" s="43"/>
     </row>
-    <row r="1090" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1090" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1090" s="19"/>
       <c r="F1090" s="19"/>
       <c r="G1090" s="19"/>
@@ -47982,7 +48031,7 @@
       <c r="W1090" s="7"/>
       <c r="X1090" s="43"/>
     </row>
-    <row r="1091" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1091" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1091" s="19"/>
       <c r="F1091" s="19"/>
       <c r="G1091" s="19"/>
@@ -48019,7 +48068,7 @@
       <c r="W1091" s="7"/>
       <c r="X1091" s="43"/>
     </row>
-    <row r="1092" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1092" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1092" s="19"/>
       <c r="F1092" s="19"/>
       <c r="G1092" s="19"/>
@@ -48056,48 +48105,50 @@
       <c r="W1092" s="7"/>
       <c r="X1092" s="43"/>
     </row>
-    <row r="1093" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="E1093" s="19"/>
-      <c r="F1093" s="19"/>
-      <c r="G1093" s="19"/>
-      <c r="H1093" s="39"/>
-      <c r="I1093" s="48" t="s">
+    <row r="1093" spans="3:24" s="72" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1093" s="69"/>
+      <c r="D1093" s="62"/>
+      <c r="E1093" s="63"/>
+      <c r="F1093" s="63"/>
+      <c r="G1093" s="63"/>
+      <c r="H1093" s="70"/>
+      <c r="I1093" s="64" t="s">
         <v>1014</v>
       </c>
-      <c r="J1093" s="46">
+      <c r="J1093" s="65">
         <v>38</v>
       </c>
-      <c r="K1093" s="16">
+      <c r="K1093" s="66">
         <f t="shared" si="37"/>
         <v>1092</v>
       </c>
-      <c r="L1093" s="5">
+      <c r="L1093" s="66">
         <f t="shared" si="37"/>
         <v>26</v>
       </c>
-      <c r="M1093" s="5">
+      <c r="M1093" s="66">
         <f t="shared" si="36"/>
         <v>26</v>
       </c>
-      <c r="N1093" s="43" t="s">
+      <c r="N1093" s="67" t="s">
         <v>490</v>
       </c>
-      <c r="O1093" s="6"/>
-      <c r="P1093" s="7" t="s">
+      <c r="O1093" s="71"/>
+      <c r="P1093" s="68" t="s">
         <v>1074</v>
       </c>
-      <c r="Q1093" s="7"/>
-      <c r="R1093" s="7"/>
-      <c r="S1093" s="7"/>
-      <c r="T1093" s="7"/>
-      <c r="U1093" s="7"/>
-      <c r="V1093" s="7"/>
-      <c r="W1093" s="7"/>
-      <c r="X1093" s="43" t="s">
+      <c r="Q1093" s="68"/>
+      <c r="R1093" s="68"/>
+      <c r="S1093" s="68"/>
+      <c r="T1093" s="68"/>
+      <c r="U1093" s="68"/>
+      <c r="V1093" s="68"/>
+      <c r="W1093" s="68"/>
+      <c r="X1093" s="67" t="s">
         <v>1083</v>
       </c>
     </row>
-    <row r="1094" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1094" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1094" s="19"/>
       <c r="F1094" s="19"/>
       <c r="G1094" s="19"/>
@@ -48132,7 +48183,7 @@
       <c r="W1094" s="7"/>
       <c r="X1094" s="43"/>
     </row>
-    <row r="1095" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1095" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1095" s="19"/>
       <c r="F1095" s="19"/>
       <c r="G1095" s="19"/>
@@ -48169,7 +48220,7 @@
       <c r="W1095" s="7"/>
       <c r="X1095" s="43"/>
     </row>
-    <row r="1096" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1096" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1096" s="19"/>
       <c r="F1096" s="19"/>
       <c r="G1096" s="19"/>
@@ -48208,7 +48259,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="1097" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1097" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1097" s="19"/>
       <c r="F1097" s="19"/>
       <c r="G1097" s="19"/>
@@ -48245,7 +48296,7 @@
       <c r="W1097" s="7"/>
       <c r="X1097" s="43"/>
     </row>
-    <row r="1098" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1098" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1098" s="19"/>
       <c r="F1098" s="19"/>
       <c r="G1098" s="19"/>
@@ -48286,7 +48337,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="1099" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1099" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1099" s="19"/>
       <c r="F1099" s="19"/>
       <c r="G1099" s="19"/>
@@ -48323,7 +48374,7 @@
       <c r="W1099" s="7"/>
       <c r="X1099" s="43"/>
     </row>
-    <row r="1100" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1100" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1100" s="19"/>
       <c r="F1100" s="19"/>
       <c r="G1100" s="19"/>
@@ -48360,7 +48411,7 @@
       <c r="W1100" s="7"/>
       <c r="X1100" s="43"/>
     </row>
-    <row r="1101" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1101" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1101" s="19"/>
       <c r="F1101" s="19"/>
       <c r="G1101" s="19"/>
@@ -48397,7 +48448,7 @@
       <c r="W1101" s="7"/>
       <c r="X1101" s="43"/>
     </row>
-    <row r="1102" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1102" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1102" s="19"/>
       <c r="F1102" s="19"/>
       <c r="G1102" s="19"/>
@@ -48436,7 +48487,7 @@
       <c r="W1102" s="7"/>
       <c r="X1102" s="43"/>
     </row>
-    <row r="1103" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1103" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1103" s="19"/>
       <c r="F1103" s="19"/>
       <c r="G1103" s="19"/>
@@ -48473,7 +48524,7 @@
       <c r="W1103" s="7"/>
       <c r="X1103" s="43"/>
     </row>
-    <row r="1104" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1104" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1104" s="19"/>
       <c r="F1104" s="19"/>
       <c r="G1104" s="19"/>
@@ -48996,7 +49047,9 @@
       <c r="R1117" s="7"/>
       <c r="S1117" s="7"/>
       <c r="T1117" s="7"/>
-      <c r="U1117" s="7"/>
+      <c r="U1117" s="7" t="s">
+        <v>1475</v>
+      </c>
       <c r="V1117" s="7"/>
       <c r="W1117" s="7"/>
       <c r="X1117" s="43"/>
@@ -49366,7 +49419,7 @@
         <v>11</v>
       </c>
       <c r="N1127" s="43" t="s">
-        <v>1431</v>
+        <v>1430</v>
       </c>
       <c r="O1127" s="7"/>
       <c r="P1127" s="7"/>
@@ -49982,7 +50035,7 @@
       <c r="V1143" s="7"/>
       <c r="W1143" s="7"/>
       <c r="X1143" s="43" t="s">
-        <v>1083</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1144" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -50976,7 +51029,7 @@
       <c r="V1169" s="7"/>
       <c r="W1169" s="7"/>
       <c r="X1169" s="43" t="s">
-        <v>1083</v>
+        <v>1476</v>
       </c>
     </row>
     <row r="1170" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -51008,12 +51061,12 @@
       <c r="Q1170" s="7"/>
       <c r="R1170" s="7"/>
       <c r="S1170" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T1170" s="7"/>
       <c r="U1170" s="7"/>
       <c r="V1170" s="7" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="W1170" s="7"/>
       <c r="X1170" s="43"/>
@@ -51208,7 +51261,7 @@
       <c r="V1175" s="7"/>
       <c r="W1175" s="7"/>
       <c r="X1175" s="43" t="s">
-        <v>1432</v>
+        <v>1431</v>
       </c>
     </row>
     <row r="1176" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -52384,12 +52437,12 @@
       <c r="Q1206" s="7"/>
       <c r="R1206" s="7"/>
       <c r="S1206" s="7" t="s">
-        <v>1461</v>
+        <v>1459</v>
       </c>
       <c r="T1206" s="7"/>
       <c r="U1206" s="7"/>
       <c r="V1206" s="7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="W1206" s="7"/>
       <c r="X1206" s="43"/>
@@ -52649,10 +52702,10 @@
       <c r="Q1213" s="7"/>
       <c r="R1213" s="7"/>
       <c r="S1213" s="7" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="T1213" s="7" t="s">
-        <v>1462</v>
+        <v>1460</v>
       </c>
       <c r="U1213" s="7"/>
       <c r="V1213" s="7"/>
@@ -53981,7 +54034,7 @@
       <c r="R1248" s="7"/>
       <c r="S1248" s="7"/>
       <c r="T1248" s="7"/>
-      <c r="U1248" s="7"/>
+      <c r="U1248" s="37"/>
       <c r="V1248" s="7"/>
       <c r="W1248" s="7"/>
       <c r="X1248" s="43"/>
@@ -54360,7 +54413,7 @@
       <c r="S1258" s="7"/>
       <c r="T1258" s="7"/>
       <c r="U1258" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V1258" s="7"/>
       <c r="W1258" s="7"/>
@@ -54927,10 +54980,10 @@
       <c r="Q1273" s="7"/>
       <c r="R1273" s="7"/>
       <c r="S1273" s="7" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="T1273" s="7" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="U1273" s="7"/>
       <c r="V1273" s="7"/>
@@ -55540,7 +55593,7 @@
       <c r="S1289" s="7"/>
       <c r="T1289" s="7"/>
       <c r="U1289" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V1289" s="7"/>
       <c r="W1289" s="7"/>
@@ -55694,7 +55747,7 @@
       <c r="S1293" s="7"/>
       <c r="T1293" s="7"/>
       <c r="U1293" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V1293" s="7"/>
       <c r="W1293" s="7"/>
@@ -56718,11 +56771,11 @@
       <c r="P1320" s="7"/>
       <c r="Q1320" s="7"/>
       <c r="R1320" s="7"/>
-      <c r="S1320" s="7" t="s">
-        <v>1439</v>
-      </c>
-      <c r="T1320" s="7" t="s">
-        <v>1442</v>
+      <c r="S1320" s="37" t="s">
+        <v>1438</v>
+      </c>
+      <c r="T1320" s="37" t="s">
+        <v>1441</v>
       </c>
       <c r="U1320" s="7"/>
       <c r="V1320" s="7"/>
@@ -56903,7 +56956,7 @@
         <v>100</v>
       </c>
       <c r="N1325" s="43" t="s">
-        <v>1433</v>
+        <v>1432</v>
       </c>
       <c r="O1325" s="6"/>
       <c r="P1325" s="7"/>
@@ -56951,7 +57004,7 @@
       <c r="S1326" s="7"/>
       <c r="T1326" s="7"/>
       <c r="U1326" s="7" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="V1326" s="7"/>
       <c r="W1326" s="7"/>
@@ -57616,7 +57669,7 @@
       <c r="V1343" s="7"/>
       <c r="W1343" s="7"/>
       <c r="X1343" s="58" t="s">
-        <v>1463</v>
+        <v>1461</v>
       </c>
     </row>
     <row r="1344" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -57956,7 +58009,7 @@
       <c r="S1352" s="7"/>
       <c r="T1352" s="7"/>
       <c r="U1352" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V1352" s="7"/>
       <c r="W1352" s="7"/>
@@ -58342,10 +58395,10 @@
       <c r="Q1362" s="7"/>
       <c r="R1362" s="7"/>
       <c r="S1362" s="37" t="s">
-        <v>1449</v>
+        <v>1447</v>
       </c>
       <c r="T1362" s="37" t="s">
-        <v>1450</v>
+        <v>1448</v>
       </c>
       <c r="U1362" s="7"/>
       <c r="V1362" s="7"/>
@@ -58526,7 +58579,7 @@
         <v>24</v>
       </c>
       <c r="N1367" s="43" t="s">
-        <v>1434</v>
+        <v>1433</v>
       </c>
       <c r="O1367" s="6" t="s">
         <v>1064</v>
@@ -59234,9 +59287,7 @@
       <c r="R1385" s="7"/>
       <c r="S1385" s="7"/>
       <c r="T1385" s="7"/>
-      <c r="U1385" s="7" t="s">
-        <v>1464</v>
-      </c>
+      <c r="U1385" s="7"/>
       <c r="V1385" s="7"/>
       <c r="W1385" s="7"/>
       <c r="X1385" s="43"/>
@@ -59465,7 +59516,7 @@
       <c r="S1391" s="7"/>
       <c r="T1391" s="7"/>
       <c r="U1391" s="7" t="s">
-        <v>1473</v>
+        <v>1470</v>
       </c>
       <c r="V1391" s="7"/>
       <c r="W1391" s="7"/>
@@ -59806,9 +59857,7 @@
       <c r="R1400" s="7"/>
       <c r="S1400" s="7"/>
       <c r="T1400" s="7"/>
-      <c r="U1400" s="7" t="s">
-        <v>1464</v>
-      </c>
+      <c r="U1400" s="7"/>
       <c r="V1400" s="7"/>
       <c r="W1400" s="7"/>
       <c r="X1400" s="43"/>
@@ -59957,7 +60006,7 @@
       <c r="S1404" s="7"/>
       <c r="T1404" s="7"/>
       <c r="U1404" s="7" t="s">
-        <v>1441</v>
+        <v>1477</v>
       </c>
       <c r="V1404" s="7"/>
       <c r="W1404" s="7"/>
@@ -60679,7 +60728,9 @@
       <c r="R1423" s="7"/>
       <c r="S1423" s="7"/>
       <c r="T1423" s="7"/>
-      <c r="U1423" s="7"/>
+      <c r="U1423" s="7" t="s">
+        <v>1454</v>
+      </c>
       <c r="V1423" s="7"/>
       <c r="W1423" s="7"/>
       <c r="X1423" s="43"/>
@@ -61062,7 +61113,7 @@
       <c r="S1433" s="7"/>
       <c r="T1433" s="7"/>
       <c r="U1433" s="7" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="V1433" s="7"/>
       <c r="W1433" s="7"/>
@@ -61440,12 +61491,12 @@
       <c r="Q1443" s="7"/>
       <c r="R1443" s="7"/>
       <c r="S1443" s="7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="T1443" s="7"/>
       <c r="U1443" s="7"/>
       <c r="V1443" s="7" t="s">
-        <v>1453</v>
+        <v>1451</v>
       </c>
       <c r="W1443" s="7"/>
       <c r="X1443" s="43"/>
@@ -61595,7 +61646,7 @@
       <c r="S1447" s="7"/>
       <c r="T1447" s="7"/>
       <c r="U1447" s="7" t="s">
-        <v>1441</v>
+        <v>1478</v>
       </c>
       <c r="V1447" s="7"/>
       <c r="W1447" s="7"/>
@@ -61641,7 +61692,7 @@
       <c r="V1448" s="7"/>
       <c r="W1448" s="7"/>
       <c r="X1448" s="56" t="s">
-        <v>1474</v>
+        <v>1471</v>
       </c>
     </row>
     <row r="1449" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -61982,7 +62033,7 @@
       <c r="V1457" s="7"/>
       <c r="W1457" s="7"/>
       <c r="X1457" s="43" t="s">
-        <v>1435</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1458" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -62512,7 +62563,7 @@
       <c r="V1471" s="7"/>
       <c r="W1471" s="7"/>
       <c r="X1471" s="43" t="s">
-        <v>1436</v>
+        <v>1435</v>
       </c>
     </row>
     <row r="1472" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -62850,10 +62901,10 @@
       <c r="Q1480" s="7"/>
       <c r="R1480" s="7"/>
       <c r="S1480" s="7" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="T1480" s="7" t="s">
-        <v>1454</v>
+        <v>1452</v>
       </c>
       <c r="U1480" s="7"/>
       <c r="V1480" s="7"/>
@@ -63607,7 +63658,7 @@
       <c r="V1500" s="7"/>
       <c r="W1500" s="7"/>
       <c r="X1500" s="56" t="s">
-        <v>1465</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1501" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -63755,11 +63806,11 @@
       <c r="P1504" s="7"/>
       <c r="Q1504" s="7"/>
       <c r="R1504" s="7"/>
-      <c r="S1504" s="7" t="s">
-        <v>1443</v>
-      </c>
-      <c r="T1504" s="7" t="s">
+      <c r="S1504" s="37" t="s">
         <v>1442</v>
+      </c>
+      <c r="T1504" s="37" t="s">
+        <v>1441</v>
       </c>
       <c r="U1504" s="7"/>
       <c r="V1504" s="7"/>
@@ -64218,10 +64269,10 @@
       <c r="Q1516" s="7"/>
       <c r="R1516" s="7"/>
       <c r="S1516" s="7" t="s">
-        <v>1439</v>
+        <v>1438</v>
       </c>
       <c r="T1516" s="7" t="s">
-        <v>1438</v>
+        <v>1437</v>
       </c>
       <c r="U1516" s="7"/>
       <c r="V1516" s="7"/>
@@ -64303,12 +64354,12 @@
       <c r="S1518" s="7"/>
       <c r="T1518" s="7"/>
       <c r="U1518" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="V1518" s="7"/>
       <c r="W1518" s="7"/>
       <c r="X1518" s="43" t="s">
-        <v>1455</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1519" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -64912,9 +64963,7 @@
       <c r="R1534" s="7"/>
       <c r="S1534" s="7"/>
       <c r="T1534" s="7"/>
-      <c r="U1534" s="7" t="s">
-        <v>1444</v>
-      </c>
+      <c r="U1534" s="7"/>
       <c r="V1534" s="7"/>
       <c r="W1534" s="7"/>
       <c r="X1534" s="43"/>
@@ -65303,7 +65352,9 @@
       <c r="R1544" s="7"/>
       <c r="S1544" s="7"/>
       <c r="T1544" s="7"/>
-      <c r="U1544" s="7"/>
+      <c r="U1544" s="7" t="s">
+        <v>1449</v>
+      </c>
       <c r="V1544" s="7"/>
       <c r="W1544" s="7"/>
       <c r="X1544" s="43" t="s">
@@ -65678,7 +65729,7 @@
       <c r="Q1554" s="7"/>
       <c r="R1554" s="7"/>
       <c r="S1554" s="7" t="s">
-        <v>1466</v>
+        <v>1463</v>
       </c>
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
@@ -65721,10 +65772,10 @@
       <c r="Q1555" s="7"/>
       <c r="R1555" s="7"/>
       <c r="S1555" s="37" t="s">
-        <v>1443</v>
+        <v>1442</v>
       </c>
       <c r="T1555" s="37" t="s">
-        <v>1442</v>
+        <v>1441</v>
       </c>
       <c r="U1555" s="7"/>
       <c r="V1555" s="7"/>
@@ -67980,7 +68031,7 @@
         <f t="shared" si="52"/>
         <v>141</v>
       </c>
-      <c r="N1632" s="62" t="s">
+      <c r="N1632" s="61" t="s">
         <v>288</v>
       </c>
       <c r="X1632" s="43"/>
@@ -68035,7 +68086,7 @@
         <v>1076</v>
       </c>
       <c r="U1634" s="1" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X1634" s="43"/>
     </row>
@@ -68140,7 +68191,7 @@
         <v>1074</v>
       </c>
       <c r="X1638" s="43" t="s">
-        <v>1467</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1639" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -68166,12 +68217,12 @@
         <v>246</v>
       </c>
       <c r="S1639" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T1639" s="7"/>
       <c r="U1639" s="7"/>
       <c r="V1639" s="7" t="s">
-        <v>1447</v>
+        <v>1445</v>
       </c>
       <c r="X1639" s="43"/>
     </row>
@@ -68197,6 +68248,9 @@
       <c r="N1640" s="43" t="s">
         <v>84</v>
       </c>
+      <c r="U1640" s="60" t="s">
+        <v>1479</v>
+      </c>
       <c r="X1640" s="43"/>
     </row>
     <row r="1641" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -68518,6 +68572,9 @@
       <c r="N1653" s="43" t="s">
         <v>292</v>
       </c>
+      <c r="U1653" s="1" t="s">
+        <v>1454</v>
+      </c>
       <c r="X1653" s="43"/>
     </row>
     <row r="1654" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -68649,7 +68706,7 @@
         <v>159</v>
       </c>
       <c r="U1658" s="1" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X1658" s="43"/>
     </row>
@@ -68729,7 +68786,7 @@
         <v>84</v>
       </c>
       <c r="U1661" s="7" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="X1661" s="43"/>
     </row>
@@ -68759,7 +68816,7 @@
         <v>1064</v>
       </c>
       <c r="U1662" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X1662" s="43" t="s">
         <v>286</v>
@@ -68791,7 +68848,7 @@
         <v>1074</v>
       </c>
       <c r="X1663" s="43" t="s">
-        <v>1475</v>
+        <v>1472</v>
       </c>
     </row>
     <row r="1664" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -68971,7 +69028,7 @@
         <v>84</v>
       </c>
       <c r="U1670" s="7" t="s">
-        <v>1451</v>
+        <v>1465</v>
       </c>
       <c r="X1670" s="43"/>
     </row>
@@ -69053,7 +69110,7 @@
         <v>278</v>
       </c>
       <c r="U1673" s="7" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="X1673" s="43"/>
     </row>
@@ -69238,7 +69295,7 @@
         <v>1074</v>
       </c>
       <c r="X1680" s="56" t="s">
-        <v>1469</v>
+        <v>1466</v>
       </c>
     </row>
     <row r="1681" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -69497,7 +69554,7 @@
         <v>1076</v>
       </c>
       <c r="U1690" s="1" t="s">
-        <v>1456</v>
+        <v>1454</v>
       </c>
       <c r="X1690" s="43"/>
     </row>
@@ -70167,8 +70224,8 @@
       <c r="P1715" s="7" t="s">
         <v>1074</v>
       </c>
-      <c r="U1715" s="7" t="s">
-        <v>1456</v>
+      <c r="U1715" s="37" t="s">
+        <v>1480</v>
       </c>
       <c r="X1715" s="43" t="s">
         <v>250</v>
@@ -70224,7 +70281,7 @@
         <v>1076</v>
       </c>
       <c r="U1717" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X1717" s="43"/>
     </row>
@@ -70355,12 +70412,12 @@
         <v>246</v>
       </c>
       <c r="S1722" s="7" t="s">
-        <v>1446</v>
+        <v>1444</v>
       </c>
       <c r="T1722" s="7"/>
       <c r="U1722" s="7"/>
       <c r="V1722" s="7" t="s">
-        <v>1452</v>
+        <v>1450</v>
       </c>
       <c r="X1722" s="43"/>
     </row>
@@ -70696,7 +70753,7 @@
         <v>84</v>
       </c>
       <c r="U1735" s="7" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="X1735" s="43"/>
     </row>
@@ -70888,7 +70945,7 @@
         <v>84</v>
       </c>
       <c r="U1742" s="7" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="X1742" s="43"/>
     </row>
@@ -71045,7 +71102,7 @@
         <v>232</v>
       </c>
       <c r="U1748" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X1748" s="43"/>
     </row>
@@ -71330,7 +71387,7 @@
         <v>84</v>
       </c>
       <c r="U1759" s="7" t="s">
-        <v>1451</v>
+        <v>1449</v>
       </c>
       <c r="X1759" s="43"/>
     </row>
@@ -71407,7 +71464,7 @@
         <v>115</v>
       </c>
       <c r="N1762" s="43" t="s">
-        <v>1437</v>
+        <v>1436</v>
       </c>
       <c r="X1762" s="43"/>
     </row>
@@ -71569,7 +71626,9 @@
       <c r="N1768" s="43" t="s">
         <v>210</v>
       </c>
-      <c r="U1768" s="7"/>
+      <c r="U1768" s="37" t="s">
+        <v>1454</v>
+      </c>
       <c r="X1768" s="43"/>
     </row>
     <row r="1769" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -71620,7 +71679,7 @@
         <v>98</v>
       </c>
       <c r="U1770" s="7" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="X1770" s="43"/>
     </row>
@@ -72314,8 +72373,8 @@
       <c r="N1797" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="U1797" s="60" t="s">
-        <v>1451</v>
+      <c r="U1797" s="1" t="s">
+        <v>1449</v>
       </c>
       <c r="X1797" s="43"/>
     </row>
@@ -72342,7 +72401,7 @@
         <v>201</v>
       </c>
       <c r="U1798" s="60" t="s">
-        <v>1441</v>
+        <v>1477</v>
       </c>
       <c r="X1798" s="43"/>
     </row>
@@ -72574,7 +72633,7 @@
         <v>84</v>
       </c>
       <c r="U1807" s="7" t="s">
-        <v>1468</v>
+        <v>1465</v>
       </c>
       <c r="X1807" s="43"/>
     </row>
@@ -72679,7 +72738,7 @@
         <v>1074</v>
       </c>
       <c r="X1811" s="43" t="s">
-        <v>1476</v>
+        <v>1473</v>
       </c>
     </row>
     <row r="1812" spans="9:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Padam template 1.3 &1.4 Rules Table 17/10/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
@@ -15,7 +15,7 @@
     <sheet name="TS 1.4" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.4'!$C$1:$X$1812</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'TS 1.4'!$C$1:$X$1811</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4739" uniqueCount="1481">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4725" uniqueCount="1475">
   <si>
     <t>Passage</t>
   </si>
@@ -4346,48 +4346,27 @@
     <t>Vis</t>
   </si>
   <si>
-    <t>s</t>
-  </si>
-  <si>
     <t>NE</t>
   </si>
   <si>
     <t>r</t>
   </si>
   <si>
-    <t>vis</t>
-  </si>
-  <si>
     <t>EL</t>
   </si>
   <si>
     <t>ngmv</t>
   </si>
   <si>
-    <t>N(gm)</t>
-  </si>
-  <si>
     <t>caqmU |</t>
   </si>
   <si>
-    <t>ntN</t>
-  </si>
-  <si>
     <t>N</t>
   </si>
   <si>
     <t>NSE</t>
   </si>
   <si>
-    <t>n(gm)</t>
-  </si>
-  <si>
-    <t>S(gg)</t>
-  </si>
-  <si>
-    <t>n(s)</t>
-  </si>
-  <si>
     <t>aqstvitya#stu ||</t>
   </si>
   <si>
@@ -4409,18 +4388,12 @@
     <t>ngmr</t>
   </si>
   <si>
-    <t>R(s)</t>
-  </si>
-  <si>
     <t>saq(gg)qskRuqtamiti# sa(gg)skRuqtam ||</t>
   </si>
   <si>
     <t>uqvityu# ||</t>
   </si>
   <si>
-    <t>??</t>
-  </si>
-  <si>
     <t>aqsRuqkShmaqhItya#sRukShmahi |</t>
   </si>
   <si>
@@ -4470,6 +4443,15 @@
   </si>
   <si>
     <t>NRE+se?</t>
+  </si>
+  <si>
+    <t>ngg</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>P</t>
   </si>
 </sst>
 </file>
@@ -4595,7 +4577,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -4611,12 +4593,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4648,7 +4624,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="73">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -4825,37 +4801,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5139,10 +5084,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1802" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="L1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="U1798" sqref="U1798"/>
+      <selection pane="bottomLeft" activeCell="T1796" sqref="T1796"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -5886,7 +5831,7 @@
       <c r="S6" s="11"/>
       <c r="T6" s="11"/>
       <c r="U6" s="11" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V6" s="11"/>
       <c r="W6" s="11"/>
@@ -8665,7 +8610,7 @@
       <c r="V73" s="11"/>
       <c r="W73" s="11"/>
       <c r="X73" s="43" t="s">
-        <v>1455</v>
+        <v>1448</v>
       </c>
     </row>
     <row r="74" spans="1:24" s="4" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
@@ -10140,9 +10085,7 @@
       <c r="S111" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T111" s="7" t="s">
-        <v>1439</v>
-      </c>
+      <c r="T111" s="7"/>
       <c r="U111" s="7"/>
       <c r="V111" s="7"/>
       <c r="W111" s="7"/>
@@ -10374,7 +10317,7 @@
       <c r="S117" s="7"/>
       <c r="T117" s="7"/>
       <c r="U117" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V117" s="7"/>
       <c r="W117" s="7"/>
@@ -10956,9 +10899,7 @@
       <c r="S132" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T132" s="7" t="s">
-        <v>1439</v>
-      </c>
+      <c r="T132" s="7"/>
       <c r="U132" s="7"/>
       <c r="V132" s="7"/>
       <c r="W132" s="7"/>
@@ -11036,9 +10977,7 @@
       <c r="S134" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T134" s="7" t="s">
-        <v>1439</v>
-      </c>
+      <c r="T134" s="7"/>
       <c r="U134" s="7"/>
       <c r="V134" s="7"/>
       <c r="W134" s="7"/>
@@ -12047,9 +11986,7 @@
       <c r="S160" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T160" s="7" t="s">
-        <v>1441</v>
-      </c>
+      <c r="T160" s="7"/>
       <c r="U160" s="7"/>
       <c r="V160" s="7"/>
       <c r="W160" s="7"/>
@@ -12437,9 +12374,7 @@
       <c r="S170" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T170" s="7" t="s">
-        <v>1441</v>
-      </c>
+      <c r="T170" s="7"/>
       <c r="U170" s="7"/>
       <c r="V170" s="7"/>
       <c r="W170" s="7"/>
@@ -12595,11 +12530,9 @@
       <c r="Q174" s="7"/>
       <c r="R174" s="7"/>
       <c r="S174" s="7" t="s">
-        <v>1442</v>
-      </c>
-      <c r="T174" s="7" t="s">
-        <v>1441</v>
-      </c>
+        <v>1438</v>
+      </c>
+      <c r="T174" s="7"/>
       <c r="U174" s="7"/>
       <c r="V174" s="7"/>
       <c r="W174" s="7"/>
@@ -13185,11 +13118,9 @@
       <c r="Q189" s="7"/>
       <c r="R189" s="7"/>
       <c r="S189" s="7" t="s">
-        <v>1442</v>
-      </c>
-      <c r="T189" s="7" t="s">
-        <v>1439</v>
-      </c>
+        <v>1438</v>
+      </c>
+      <c r="T189" s="7"/>
       <c r="U189" s="7"/>
       <c r="V189" s="7"/>
       <c r="W189" s="7"/>
@@ -13267,9 +13198,7 @@
       <c r="S191" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T191" s="7" t="s">
-        <v>1439</v>
-      </c>
+      <c r="T191" s="7"/>
       <c r="U191" s="7"/>
       <c r="V191" s="7"/>
       <c r="W191" s="7"/>
@@ -14681,7 +14610,7 @@
       <c r="S227" s="7"/>
       <c r="T227" s="7"/>
       <c r="U227" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V227" s="7"/>
       <c r="W227" s="7"/>
@@ -17131,7 +17060,7 @@
       <c r="S289" s="7"/>
       <c r="T289" s="7"/>
       <c r="U289" s="37" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V289" s="7"/>
       <c r="W289" s="7"/>
@@ -17881,7 +17810,7 @@
       <c r="S308" s="7"/>
       <c r="T308" s="7"/>
       <c r="U308" s="37" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V308" s="7"/>
       <c r="W308" s="7"/>
@@ -18077,7 +18006,7 @@
       <c r="S313" s="7"/>
       <c r="T313" s="7"/>
       <c r="U313" s="37" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V313" s="7"/>
       <c r="W313" s="7"/>
@@ -21203,7 +21132,7 @@
       <c r="S393" s="7"/>
       <c r="T393" s="7"/>
       <c r="U393" s="7" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V393" s="7"/>
       <c r="W393" s="7"/>
@@ -22239,7 +22168,7 @@
       <c r="S420" s="7"/>
       <c r="T420" s="7"/>
       <c r="U420" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V420" s="7"/>
       <c r="W420" s="7"/>
@@ -22831,7 +22760,7 @@
       <c r="S435" s="7"/>
       <c r="T435" s="7"/>
       <c r="U435" s="7" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V435" s="7"/>
       <c r="W435" s="7"/>
@@ -24371,7 +24300,7 @@
       <c r="S475" s="7"/>
       <c r="T475" s="7"/>
       <c r="U475" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V475" s="7"/>
       <c r="W475" s="7"/>
@@ -29663,7 +29592,7 @@
       <c r="S611" s="7"/>
       <c r="T611" s="7"/>
       <c r="U611" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V611" s="7"/>
       <c r="W611" s="7"/>
@@ -30523,12 +30452,12 @@
       <c r="Q633" s="7"/>
       <c r="R633" s="7"/>
       <c r="S633" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T633" s="7"/>
       <c r="U633" s="7"/>
       <c r="V633" s="7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="W633" s="7"/>
       <c r="X633" s="43"/>
@@ -30679,7 +30608,7 @@
       <c r="Q637" s="7"/>
       <c r="R637" s="7"/>
       <c r="S637" s="7" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="T637" s="7"/>
       <c r="U637" s="7"/>
@@ -31655,12 +31584,12 @@
       <c r="Q662" s="7"/>
       <c r="R662" s="7"/>
       <c r="S662" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T662" s="7"/>
       <c r="U662" s="7"/>
       <c r="V662" s="7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="W662" s="7"/>
       <c r="X662" s="43"/>
@@ -31851,12 +31780,12 @@
       <c r="Q667" s="7"/>
       <c r="R667" s="7"/>
       <c r="S667" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T667" s="7"/>
       <c r="U667" s="7"/>
       <c r="V667" s="7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="W667" s="7"/>
       <c r="X667" s="43" t="s">
@@ -32395,12 +32324,12 @@
       <c r="Q681" s="7"/>
       <c r="R681" s="7"/>
       <c r="S681" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T681" s="7"/>
       <c r="U681" s="7"/>
       <c r="V681" s="7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="W681" s="7"/>
       <c r="X681" s="43"/>
@@ -33677,7 +33606,7 @@
       <c r="V714" s="7"/>
       <c r="W714" s="7"/>
       <c r="X714" s="43" t="s">
-        <v>1467</v>
+        <v>1458</v>
       </c>
     </row>
     <row r="715" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -34546,7 +34475,7 @@
         <v>31</v>
       </c>
       <c r="N737" s="43" t="s">
-        <v>1474</v>
+        <v>1465</v>
       </c>
       <c r="O737" s="6" t="s">
         <v>1075</v>
@@ -35159,7 +35088,7 @@
       <c r="Q753" s="7"/>
       <c r="R753" s="7"/>
       <c r="S753" s="7" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="T753" s="7"/>
       <c r="U753" s="7"/>
@@ -35205,7 +35134,7 @@
       <c r="V754" s="7"/>
       <c r="W754" s="7"/>
       <c r="X754" s="43" t="s">
-        <v>1468</v>
+        <v>1459</v>
       </c>
     </row>
     <row r="755" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -36408,9 +36337,7 @@
       <c r="S786" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T786" s="7" t="s">
-        <v>1441</v>
-      </c>
+      <c r="T786" s="7"/>
       <c r="U786" s="7"/>
       <c r="V786" s="7"/>
       <c r="W786" s="7"/>
@@ -37288,11 +37215,11 @@
       <c r="P809" s="7"/>
       <c r="Q809" s="7"/>
       <c r="R809" s="7"/>
-      <c r="S809" s="37" t="s">
-        <v>1442</v>
+      <c r="S809" s="7" t="s">
+        <v>1438</v>
       </c>
       <c r="T809" s="37" t="s">
-        <v>1469</v>
+        <v>1460</v>
       </c>
       <c r="U809" s="7"/>
       <c r="V809" s="7"/>
@@ -37751,7 +37678,7 @@
       <c r="Q821" s="7"/>
       <c r="R821" s="7"/>
       <c r="S821" s="7" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="T821" s="7"/>
       <c r="U821" s="7"/>
@@ -37868,7 +37795,7 @@
       <c r="S824" s="7"/>
       <c r="T824" s="7"/>
       <c r="U824" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V824" s="7"/>
       <c r="W824" s="7"/>
@@ -39204,7 +39131,7 @@
         <v>3</v>
       </c>
       <c r="N859" s="43" t="s">
-        <v>1456</v>
+        <v>1449</v>
       </c>
       <c r="O859" s="6"/>
       <c r="P859" s="7"/>
@@ -39216,7 +39143,7 @@
       <c r="V859" s="7"/>
       <c r="W859" s="7"/>
       <c r="X859" s="56" t="s">
-        <v>1457</v>
+        <v>1450</v>
       </c>
     </row>
     <row r="860" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -41766,7 +41693,7 @@
       <c r="S926" s="7"/>
       <c r="T926" s="7"/>
       <c r="U926" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V926" s="7"/>
       <c r="W926" s="7"/>
@@ -41872,7 +41799,7 @@
         <v>9</v>
       </c>
       <c r="N929" s="43" t="s">
-        <v>1446</v>
+        <v>1443</v>
       </c>
       <c r="O929" s="6" t="s">
         <v>1075</v>
@@ -43370,7 +43297,7 @@
       <c r="Q968" s="7"/>
       <c r="R968" s="7"/>
       <c r="S968" s="7" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="T968" s="7"/>
       <c r="U968" s="7"/>
@@ -43834,7 +43761,7 @@
       <c r="Q980" s="7"/>
       <c r="R980" s="7"/>
       <c r="S980" s="7" t="s">
-        <v>1443</v>
+        <v>1441</v>
       </c>
       <c r="T980" s="7"/>
       <c r="U980" s="7"/>
@@ -43953,7 +43880,7 @@
       <c r="S983" s="7"/>
       <c r="T983" s="7"/>
       <c r="U983" s="7" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V983" s="7"/>
       <c r="W983" s="7"/>
@@ -43997,7 +43924,7 @@
       <c r="V984" s="7"/>
       <c r="W984" s="7"/>
       <c r="X984" s="44" t="s">
-        <v>1458</v>
+        <v>1451</v>
       </c>
     </row>
     <row r="985" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -44144,7 +44071,7 @@
       <c r="S988" s="7"/>
       <c r="T988" s="7"/>
       <c r="U988" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V988" s="7"/>
       <c r="W988" s="7"/>
@@ -47957,7 +47884,7 @@
       <c r="W1088" s="7"/>
       <c r="X1088" s="43"/>
     </row>
-    <row r="1089" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1089" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1089" s="19"/>
       <c r="F1089" s="19"/>
       <c r="G1089" s="19"/>
@@ -47994,7 +47921,7 @@
       <c r="W1089" s="7"/>
       <c r="X1089" s="43"/>
     </row>
-    <row r="1090" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1090" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1090" s="19"/>
       <c r="F1090" s="19"/>
       <c r="G1090" s="19"/>
@@ -48031,7 +47958,7 @@
       <c r="W1090" s="7"/>
       <c r="X1090" s="43"/>
     </row>
-    <row r="1091" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1091" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1091" s="19"/>
       <c r="F1091" s="19"/>
       <c r="G1091" s="19"/>
@@ -48068,7 +47995,7 @@
       <c r="W1091" s="7"/>
       <c r="X1091" s="43"/>
     </row>
-    <row r="1092" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1092" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1092" s="19"/>
       <c r="F1092" s="19"/>
       <c r="G1092" s="19"/>
@@ -48105,50 +48032,48 @@
       <c r="W1092" s="7"/>
       <c r="X1092" s="43"/>
     </row>
-    <row r="1093" spans="3:24" s="72" customFormat="1" ht="20.25" x14ac:dyDescent="0.25">
-      <c r="C1093" s="69"/>
-      <c r="D1093" s="62"/>
-      <c r="E1093" s="63"/>
-      <c r="F1093" s="63"/>
-      <c r="G1093" s="63"/>
-      <c r="H1093" s="70"/>
-      <c r="I1093" s="64" t="s">
+    <row r="1093" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="E1093" s="19"/>
+      <c r="F1093" s="19"/>
+      <c r="G1093" s="19"/>
+      <c r="H1093" s="39"/>
+      <c r="I1093" s="55" t="s">
         <v>1014</v>
       </c>
-      <c r="J1093" s="65">
+      <c r="J1093" s="46">
         <v>38</v>
       </c>
-      <c r="K1093" s="66">
+      <c r="K1093" s="5">
         <f t="shared" si="37"/>
         <v>1092</v>
       </c>
-      <c r="L1093" s="66">
+      <c r="L1093" s="5">
         <f t="shared" si="37"/>
         <v>26</v>
       </c>
-      <c r="M1093" s="66">
+      <c r="M1093" s="5">
         <f t="shared" si="36"/>
         <v>26</v>
       </c>
-      <c r="N1093" s="67" t="s">
+      <c r="N1093" s="56" t="s">
         <v>490</v>
       </c>
-      <c r="O1093" s="71"/>
-      <c r="P1093" s="68" t="s">
+      <c r="O1093" s="33"/>
+      <c r="P1093" s="7" t="s">
         <v>1074</v>
       </c>
-      <c r="Q1093" s="68"/>
-      <c r="R1093" s="68"/>
-      <c r="S1093" s="68"/>
-      <c r="T1093" s="68"/>
-      <c r="U1093" s="68"/>
-      <c r="V1093" s="68"/>
-      <c r="W1093" s="68"/>
-      <c r="X1093" s="67" t="s">
+      <c r="Q1093" s="7"/>
+      <c r="R1093" s="7"/>
+      <c r="S1093" s="7"/>
+      <c r="T1093" s="7"/>
+      <c r="U1093" s="7"/>
+      <c r="V1093" s="7"/>
+      <c r="W1093" s="7"/>
+      <c r="X1093" s="56" t="s">
         <v>1083</v>
       </c>
     </row>
-    <row r="1094" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1094" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1094" s="19"/>
       <c r="F1094" s="19"/>
       <c r="G1094" s="19"/>
@@ -48183,7 +48108,7 @@
       <c r="W1094" s="7"/>
       <c r="X1094" s="43"/>
     </row>
-    <row r="1095" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1095" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1095" s="19"/>
       <c r="F1095" s="19"/>
       <c r="G1095" s="19"/>
@@ -48220,7 +48145,7 @@
       <c r="W1095" s="7"/>
       <c r="X1095" s="43"/>
     </row>
-    <row r="1096" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1096" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1096" s="19"/>
       <c r="F1096" s="19"/>
       <c r="G1096" s="19"/>
@@ -48259,7 +48184,7 @@
         <v>1263</v>
       </c>
     </row>
-    <row r="1097" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1097" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1097" s="19"/>
       <c r="F1097" s="19"/>
       <c r="G1097" s="19"/>
@@ -48296,7 +48221,7 @@
       <c r="W1097" s="7"/>
       <c r="X1097" s="43"/>
     </row>
-    <row r="1098" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1098" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1098" s="19"/>
       <c r="F1098" s="19"/>
       <c r="G1098" s="19"/>
@@ -48337,7 +48262,7 @@
         <v>537</v>
       </c>
     </row>
-    <row r="1099" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1099" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1099" s="19"/>
       <c r="F1099" s="19"/>
       <c r="G1099" s="19"/>
@@ -48374,7 +48299,7 @@
       <c r="W1099" s="7"/>
       <c r="X1099" s="43"/>
     </row>
-    <row r="1100" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1100" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1100" s="19"/>
       <c r="F1100" s="19"/>
       <c r="G1100" s="19"/>
@@ -48411,7 +48336,7 @@
       <c r="W1100" s="7"/>
       <c r="X1100" s="43"/>
     </row>
-    <row r="1101" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1101" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1101" s="19"/>
       <c r="F1101" s="19"/>
       <c r="G1101" s="19"/>
@@ -48448,7 +48373,7 @@
       <c r="W1101" s="7"/>
       <c r="X1101" s="43"/>
     </row>
-    <row r="1102" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1102" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1102" s="19"/>
       <c r="F1102" s="19"/>
       <c r="G1102" s="19"/>
@@ -48487,7 +48412,7 @@
       <c r="W1102" s="7"/>
       <c r="X1102" s="43"/>
     </row>
-    <row r="1103" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1103" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1103" s="19"/>
       <c r="F1103" s="19"/>
       <c r="G1103" s="19"/>
@@ -48524,7 +48449,7 @@
       <c r="W1103" s="7"/>
       <c r="X1103" s="43"/>
     </row>
-    <row r="1104" spans="3:24" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1104" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
       <c r="E1104" s="19"/>
       <c r="F1104" s="19"/>
       <c r="G1104" s="19"/>
@@ -49047,8 +48972,8 @@
       <c r="R1117" s="7"/>
       <c r="S1117" s="7"/>
       <c r="T1117" s="7"/>
-      <c r="U1117" s="7" t="s">
-        <v>1475</v>
+      <c r="U1117" s="37" t="s">
+        <v>1466</v>
       </c>
       <c r="V1117" s="7"/>
       <c r="W1117" s="7"/>
@@ -50035,7 +49960,7 @@
       <c r="V1143" s="7"/>
       <c r="W1143" s="7"/>
       <c r="X1143" s="43" t="s">
-        <v>1476</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1144" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -51029,7 +50954,7 @@
       <c r="V1169" s="7"/>
       <c r="W1169" s="7"/>
       <c r="X1169" s="43" t="s">
-        <v>1476</v>
+        <v>1467</v>
       </c>
     </row>
     <row r="1170" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -51061,12 +50986,12 @@
       <c r="Q1170" s="7"/>
       <c r="R1170" s="7"/>
       <c r="S1170" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T1170" s="7"/>
       <c r="U1170" s="7"/>
       <c r="V1170" s="7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="W1170" s="7"/>
       <c r="X1170" s="43"/>
@@ -52437,12 +52362,12 @@
       <c r="Q1206" s="7"/>
       <c r="R1206" s="7"/>
       <c r="S1206" s="7" t="s">
-        <v>1459</v>
+        <v>1452</v>
       </c>
       <c r="T1206" s="7"/>
       <c r="U1206" s="7"/>
       <c r="V1206" s="7" t="s">
-        <v>1450</v>
+        <v>1444</v>
       </c>
       <c r="W1206" s="7"/>
       <c r="X1206" s="43"/>
@@ -52702,11 +52627,9 @@
       <c r="Q1213" s="7"/>
       <c r="R1213" s="7"/>
       <c r="S1213" s="7" t="s">
-        <v>1442</v>
-      </c>
-      <c r="T1213" s="7" t="s">
-        <v>1460</v>
-      </c>
+        <v>1438</v>
+      </c>
+      <c r="T1213" s="7"/>
       <c r="U1213" s="7"/>
       <c r="V1213" s="7"/>
       <c r="W1213" s="7"/>
@@ -54413,7 +54336,7 @@
       <c r="S1258" s="7"/>
       <c r="T1258" s="7"/>
       <c r="U1258" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V1258" s="7"/>
       <c r="W1258" s="7"/>
@@ -54982,9 +54905,7 @@
       <c r="S1273" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T1273" s="7" t="s">
-        <v>1441</v>
-      </c>
+      <c r="T1273" s="37"/>
       <c r="U1273" s="7"/>
       <c r="V1273" s="7"/>
       <c r="W1273" s="7"/>
@@ -55593,7 +55514,7 @@
       <c r="S1289" s="7"/>
       <c r="T1289" s="7"/>
       <c r="U1289" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V1289" s="7"/>
       <c r="W1289" s="7"/>
@@ -55747,7 +55668,7 @@
       <c r="S1293" s="7"/>
       <c r="T1293" s="7"/>
       <c r="U1293" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V1293" s="7"/>
       <c r="W1293" s="7"/>
@@ -56771,11 +56692,11 @@
       <c r="P1320" s="7"/>
       <c r="Q1320" s="7"/>
       <c r="R1320" s="7"/>
-      <c r="S1320" s="37" t="s">
+      <c r="S1320" s="7" t="s">
         <v>1438</v>
       </c>
       <c r="T1320" s="37" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="U1320" s="7"/>
       <c r="V1320" s="7"/>
@@ -57004,7 +56925,7 @@
       <c r="S1326" s="7"/>
       <c r="T1326" s="7"/>
       <c r="U1326" s="7" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V1326" s="7"/>
       <c r="W1326" s="7"/>
@@ -57669,7 +57590,7 @@
       <c r="V1343" s="7"/>
       <c r="W1343" s="7"/>
       <c r="X1343" s="58" t="s">
-        <v>1461</v>
+        <v>1453</v>
       </c>
     </row>
     <row r="1344" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -58009,7 +57930,7 @@
       <c r="S1352" s="7"/>
       <c r="T1352" s="7"/>
       <c r="U1352" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V1352" s="7"/>
       <c r="W1352" s="7"/>
@@ -58395,10 +58316,10 @@
       <c r="Q1362" s="7"/>
       <c r="R1362" s="7"/>
       <c r="S1362" s="37" t="s">
-        <v>1447</v>
+        <v>1444</v>
       </c>
       <c r="T1362" s="37" t="s">
-        <v>1448</v>
+        <v>1474</v>
       </c>
       <c r="U1362" s="7"/>
       <c r="V1362" s="7"/>
@@ -59515,8 +59436,8 @@
       <c r="R1391" s="7"/>
       <c r="S1391" s="7"/>
       <c r="T1391" s="7"/>
-      <c r="U1391" s="7" t="s">
-        <v>1470</v>
+      <c r="U1391" s="37" t="s">
+        <v>1461</v>
       </c>
       <c r="V1391" s="7"/>
       <c r="W1391" s="7"/>
@@ -60006,7 +59927,7 @@
       <c r="S1404" s="7"/>
       <c r="T1404" s="7"/>
       <c r="U1404" s="7" t="s">
-        <v>1477</v>
+        <v>1468</v>
       </c>
       <c r="V1404" s="7"/>
       <c r="W1404" s="7"/>
@@ -60729,7 +60650,7 @@
       <c r="S1423" s="7"/>
       <c r="T1423" s="7"/>
       <c r="U1423" s="7" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="V1423" s="7"/>
       <c r="W1423" s="7"/>
@@ -61113,7 +61034,7 @@
       <c r="S1433" s="7"/>
       <c r="T1433" s="7"/>
       <c r="U1433" s="7" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="V1433" s="7"/>
       <c r="W1433" s="7"/>
@@ -61491,12 +61412,12 @@
       <c r="Q1443" s="7"/>
       <c r="R1443" s="7"/>
       <c r="S1443" s="7" t="s">
-        <v>1450</v>
+        <v>1472</v>
       </c>
       <c r="T1443" s="7"/>
       <c r="U1443" s="7"/>
       <c r="V1443" s="7" t="s">
-        <v>1451</v>
+        <v>1473</v>
       </c>
       <c r="W1443" s="7"/>
       <c r="X1443" s="43"/>
@@ -61646,7 +61567,7 @@
       <c r="S1447" s="7"/>
       <c r="T1447" s="7"/>
       <c r="U1447" s="7" t="s">
-        <v>1478</v>
+        <v>1469</v>
       </c>
       <c r="V1447" s="7"/>
       <c r="W1447" s="7"/>
@@ -61692,7 +61613,7 @@
       <c r="V1448" s="7"/>
       <c r="W1448" s="7"/>
       <c r="X1448" s="56" t="s">
-        <v>1471</v>
+        <v>1462</v>
       </c>
     </row>
     <row r="1449" spans="5:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -62903,9 +62824,7 @@
       <c r="S1480" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T1480" s="7" t="s">
-        <v>1452</v>
-      </c>
+      <c r="T1480" s="7"/>
       <c r="U1480" s="7"/>
       <c r="V1480" s="7"/>
       <c r="W1480" s="7"/>
@@ -63658,7 +63577,7 @@
       <c r="V1500" s="7"/>
       <c r="W1500" s="7"/>
       <c r="X1500" s="56" t="s">
-        <v>1462</v>
+        <v>1454</v>
       </c>
     </row>
     <row r="1501" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -63806,11 +63725,11 @@
       <c r="P1504" s="7"/>
       <c r="Q1504" s="7"/>
       <c r="R1504" s="7"/>
-      <c r="S1504" s="37" t="s">
-        <v>1442</v>
+      <c r="S1504" s="7" t="s">
+        <v>1438</v>
       </c>
       <c r="T1504" s="37" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="U1504" s="7"/>
       <c r="V1504" s="7"/>
@@ -64271,9 +64190,7 @@
       <c r="S1516" s="7" t="s">
         <v>1438</v>
       </c>
-      <c r="T1516" s="7" t="s">
-        <v>1437</v>
-      </c>
+      <c r="T1516" s="7"/>
       <c r="U1516" s="7"/>
       <c r="V1516" s="7"/>
       <c r="W1516" s="7"/>
@@ -64354,12 +64271,12 @@
       <c r="S1518" s="7"/>
       <c r="T1518" s="7"/>
       <c r="U1518" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="V1518" s="7"/>
       <c r="W1518" s="7"/>
       <c r="X1518" s="43" t="s">
-        <v>1453</v>
+        <v>1446</v>
       </c>
     </row>
     <row r="1519" spans="4:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -65353,7 +65270,7 @@
       <c r="S1544" s="7"/>
       <c r="T1544" s="7"/>
       <c r="U1544" s="7" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="V1544" s="7"/>
       <c r="W1544" s="7"/>
@@ -65728,9 +65645,7 @@
       <c r="P1554" s="7"/>
       <c r="Q1554" s="7"/>
       <c r="R1554" s="7"/>
-      <c r="S1554" s="7" t="s">
-        <v>1463</v>
-      </c>
+      <c r="S1554" s="7"/>
       <c r="T1554" s="7"/>
       <c r="U1554" s="7"/>
       <c r="V1554" s="7"/>
@@ -65771,11 +65686,11 @@
       </c>
       <c r="Q1555" s="7"/>
       <c r="R1555" s="7"/>
-      <c r="S1555" s="37" t="s">
-        <v>1442</v>
+      <c r="S1555" s="7" t="s">
+        <v>1438</v>
       </c>
       <c r="T1555" s="37" t="s">
-        <v>1441</v>
+        <v>1440</v>
       </c>
       <c r="U1555" s="7"/>
       <c r="V1555" s="7"/>
@@ -68086,7 +68001,7 @@
         <v>1076</v>
       </c>
       <c r="U1634" s="1" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X1634" s="43"/>
     </row>
@@ -68191,7 +68106,7 @@
         <v>1074</v>
       </c>
       <c r="X1638" s="43" t="s">
-        <v>1464</v>
+        <v>1455</v>
       </c>
     </row>
     <row r="1639" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -68217,12 +68132,12 @@
         <v>246</v>
       </c>
       <c r="S1639" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T1639" s="7"/>
       <c r="U1639" s="7"/>
       <c r="V1639" s="7" t="s">
-        <v>1445</v>
+        <v>1444</v>
       </c>
       <c r="X1639" s="43"/>
     </row>
@@ -68249,7 +68164,7 @@
         <v>84</v>
       </c>
       <c r="U1640" s="60" t="s">
-        <v>1479</v>
+        <v>1470</v>
       </c>
       <c r="X1640" s="43"/>
     </row>
@@ -68572,8 +68487,8 @@
       <c r="N1653" s="43" t="s">
         <v>292</v>
       </c>
-      <c r="U1653" s="1" t="s">
-        <v>1454</v>
+      <c r="U1653" s="7" t="s">
+        <v>1447</v>
       </c>
       <c r="X1653" s="43"/>
     </row>
@@ -68705,8 +68620,8 @@
       <c r="N1658" s="43" t="s">
         <v>159</v>
       </c>
-      <c r="U1658" s="1" t="s">
-        <v>1440</v>
+      <c r="U1658" s="7" t="s">
+        <v>1439</v>
       </c>
       <c r="X1658" s="43"/>
     </row>
@@ -68786,7 +68701,7 @@
         <v>84</v>
       </c>
       <c r="U1661" s="7" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="X1661" s="43"/>
     </row>
@@ -68816,7 +68731,7 @@
         <v>1064</v>
       </c>
       <c r="U1662" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X1662" s="43" t="s">
         <v>286</v>
@@ -68848,7 +68763,7 @@
         <v>1074</v>
       </c>
       <c r="X1663" s="43" t="s">
-        <v>1472</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1664" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -69028,7 +68943,7 @@
         <v>84</v>
       </c>
       <c r="U1670" s="7" t="s">
-        <v>1465</v>
+        <v>1456</v>
       </c>
       <c r="X1670" s="43"/>
     </row>
@@ -69110,7 +69025,7 @@
         <v>278</v>
       </c>
       <c r="U1673" s="7" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="X1673" s="43"/>
     </row>
@@ -69295,7 +69210,7 @@
         <v>1074</v>
       </c>
       <c r="X1680" s="56" t="s">
-        <v>1466</v>
+        <v>1457</v>
       </c>
     </row>
     <row r="1681" spans="9:24" ht="20.25" x14ac:dyDescent="0.25">
@@ -69554,7 +69469,7 @@
         <v>1076</v>
       </c>
       <c r="U1690" s="1" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="X1690" s="43"/>
     </row>
@@ -70225,7 +70140,7 @@
         <v>1074</v>
       </c>
       <c r="U1715" s="37" t="s">
-        <v>1480</v>
+        <v>1471</v>
       </c>
       <c r="X1715" s="43" t="s">
         <v>250</v>
@@ -70281,7 +70196,7 @@
         <v>1076</v>
       </c>
       <c r="U1717" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X1717" s="43"/>
     </row>
@@ -70412,12 +70327,12 @@
         <v>246</v>
       </c>
       <c r="S1722" s="7" t="s">
-        <v>1444</v>
+        <v>1442</v>
       </c>
       <c r="T1722" s="7"/>
       <c r="U1722" s="7"/>
       <c r="V1722" s="7" t="s">
-        <v>1450</v>
+        <v>1444</v>
       </c>
       <c r="X1722" s="43"/>
     </row>
@@ -70753,7 +70668,7 @@
         <v>84</v>
       </c>
       <c r="U1735" s="7" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="X1735" s="43"/>
     </row>
@@ -70945,7 +70860,7 @@
         <v>84</v>
       </c>
       <c r="U1742" s="7" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="X1742" s="43"/>
     </row>
@@ -71102,7 +71017,7 @@
         <v>232</v>
       </c>
       <c r="U1748" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X1748" s="43"/>
     </row>
@@ -71387,7 +71302,7 @@
         <v>84</v>
       </c>
       <c r="U1759" s="7" t="s">
-        <v>1449</v>
+        <v>1445</v>
       </c>
       <c r="X1759" s="43"/>
     </row>
@@ -71627,7 +71542,7 @@
         <v>210</v>
       </c>
       <c r="U1768" s="37" t="s">
-        <v>1454</v>
+        <v>1447</v>
       </c>
       <c r="X1768" s="43"/>
     </row>
@@ -71679,7 +71594,7 @@
         <v>98</v>
       </c>
       <c r="U1770" s="7" t="s">
-        <v>1440</v>
+        <v>1439</v>
       </c>
       <c r="X1770" s="43"/>
     </row>
@@ -72373,8 +72288,8 @@
       <c r="N1797" s="43" t="s">
         <v>84</v>
       </c>
-      <c r="U1797" s="1" t="s">
-        <v>1449</v>
+      <c r="U1797" s="7" t="s">
+        <v>1445</v>
       </c>
       <c r="X1797" s="43"/>
     </row>
@@ -72400,8 +72315,8 @@
       <c r="N1798" s="43" t="s">
         <v>201</v>
       </c>
-      <c r="U1798" s="60" t="s">
-        <v>1477</v>
+      <c r="U1798" s="37" t="s">
+        <v>1468</v>
       </c>
       <c r="X1798" s="43"/>
     </row>
@@ -72633,7 +72548,7 @@
         <v>84</v>
       </c>
       <c r="U1807" s="7" t="s">
-        <v>1465</v>
+        <v>1456</v>
       </c>
       <c r="X1807" s="43"/>
     </row>
@@ -72738,7 +72653,7 @@
         <v>1074</v>
       </c>
       <c r="X1811" s="43" t="s">
-        <v>1473</v>
+        <v>1464</v>
       </c>
     </row>
     <row r="1812" spans="9:24" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
GS Padam template updates 05/12/2020
</commit_message>
<xml_diff>
--- a/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
+++ b/TS Jatai Working/Raja Files/Padam Inputs/TS 1.4 Padam Input Template.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5146" uniqueCount="1488">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5310" uniqueCount="1488">
   <si>
     <t>Passage</t>
   </si>
@@ -4497,13 +4497,19 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="20" x14ac:knownFonts="1">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="14"/>
@@ -4662,182 +4668,185 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="17" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="17" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="16" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="17" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="15" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="11" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="10" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="49" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="16" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -5125,10 +5134,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:V1812"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A1736" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A1800" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="L1" sqref="L1"/>
-      <selection pane="bottomLeft" activeCell="E1491" sqref="E1491"/>
+      <selection pane="bottomLeft" activeCell="C1649" sqref="C1649:C1811"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.25"/>
@@ -65752,7 +65761,7 @@
       </c>
       <c r="V1632" s="42"/>
     </row>
-    <row r="1633" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1633" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1633" s="47" t="s">
         <v>23</v>
       </c>
@@ -65776,7 +65785,7 @@
       </c>
       <c r="V1633" s="42"/>
     </row>
-    <row r="1634" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1634" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1634" s="47" t="s">
         <v>23</v>
       </c>
@@ -65806,7 +65815,7 @@
       </c>
       <c r="V1634" s="42"/>
     </row>
-    <row r="1635" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1635" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1635" s="47" t="s">
         <v>23</v>
       </c>
@@ -65830,7 +65839,7 @@
       </c>
       <c r="V1635" s="42"/>
     </row>
-    <row r="1636" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1636" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1636" s="47" t="s">
         <v>23</v>
       </c>
@@ -65854,7 +65863,7 @@
       </c>
       <c r="V1636" s="42"/>
     </row>
-    <row r="1637" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1637" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1637" s="47" t="s">
         <v>23</v>
       </c>
@@ -65881,7 +65890,7 @@
       </c>
       <c r="V1637" s="42"/>
     </row>
-    <row r="1638" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1638" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1638" s="47" t="s">
         <v>23</v>
       </c>
@@ -65910,7 +65919,7 @@
         <v>1343</v>
       </c>
     </row>
-    <row r="1639" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1639" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1639" s="47" t="s">
         <v>23</v>
       </c>
@@ -65941,7 +65950,7 @@
       <c r="U1639" s="7"/>
       <c r="V1639" s="42"/>
     </row>
-    <row r="1640" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1640" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1640" s="47" t="s">
         <v>23</v>
       </c>
@@ -65965,7 +65974,7 @@
       </c>
       <c r="V1640" s="42"/>
     </row>
-    <row r="1641" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1641" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1641" s="47" t="s">
         <v>23</v>
       </c>
@@ -65992,7 +66001,7 @@
       </c>
       <c r="V1641" s="42"/>
     </row>
-    <row r="1642" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1642" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1642" s="47" t="s">
         <v>23</v>
       </c>
@@ -66016,7 +66025,7 @@
       </c>
       <c r="V1642" s="42"/>
     </row>
-    <row r="1643" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1643" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1643" s="47" t="s">
         <v>23</v>
       </c>
@@ -66040,7 +66049,7 @@
       </c>
       <c r="V1643" s="42"/>
     </row>
-    <row r="1644" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1644" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1644" s="47" t="s">
         <v>23</v>
       </c>
@@ -66064,7 +66073,7 @@
       </c>
       <c r="V1644" s="42"/>
     </row>
-    <row r="1645" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1645" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1645" s="47" t="s">
         <v>23</v>
       </c>
@@ -66091,7 +66100,7 @@
       </c>
       <c r="V1645" s="42"/>
     </row>
-    <row r="1646" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1646" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1646" s="47" t="s">
         <v>23</v>
       </c>
@@ -66115,7 +66124,7 @@
       </c>
       <c r="V1646" s="42"/>
     </row>
-    <row r="1647" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1647" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
       <c r="I1647" s="47" t="s">
         <v>23</v>
       </c>
@@ -66144,7 +66153,10 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="1648" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1648" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1648" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1648" s="59" t="s">
         <v>141</v>
       </c>
@@ -66169,7 +66181,10 @@
       </c>
       <c r="V1648" s="42"/>
     </row>
-    <row r="1649" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1649" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1649" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1649" s="59" t="s">
         <v>141</v>
       </c>
@@ -66196,7 +66211,10 @@
       </c>
       <c r="V1649" s="42"/>
     </row>
-    <row r="1650" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1650" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1650" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1650" s="47" t="s">
         <v>22</v>
       </c>
@@ -66220,7 +66238,10 @@
       </c>
       <c r="V1650" s="42"/>
     </row>
-    <row r="1651" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1651" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1651" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1651" s="47" t="s">
         <v>22</v>
       </c>
@@ -66244,7 +66265,10 @@
       </c>
       <c r="V1651" s="42"/>
     </row>
-    <row r="1652" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1652" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1652" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1652" s="59" t="s">
         <v>142</v>
       </c>
@@ -66271,7 +66295,10 @@
       </c>
       <c r="V1652" s="42"/>
     </row>
-    <row r="1653" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1653" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1653" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1653" s="59" t="s">
         <v>142</v>
       </c>
@@ -66301,7 +66328,10 @@
       </c>
       <c r="V1653" s="42"/>
     </row>
-    <row r="1654" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1654" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1654" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1654" s="59" t="s">
         <v>142</v>
       </c>
@@ -66328,7 +66358,10 @@
       </c>
       <c r="V1654" s="42"/>
     </row>
-    <row r="1655" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1655" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1655" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1655" s="59" t="s">
         <v>142</v>
       </c>
@@ -66360,7 +66393,10 @@
         <v>1354</v>
       </c>
     </row>
-    <row r="1656" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1656" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1656" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1656" s="47" t="s">
         <v>22</v>
       </c>
@@ -66389,7 +66425,10 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1657" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1657" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1657" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1657" s="47" t="s">
         <v>22</v>
       </c>
@@ -66413,7 +66452,10 @@
       </c>
       <c r="V1657" s="42"/>
     </row>
-    <row r="1658" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1658" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1658" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1658" s="47" t="s">
         <v>22</v>
       </c>
@@ -66440,7 +66482,10 @@
       </c>
       <c r="V1658" s="42"/>
     </row>
-    <row r="1659" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1659" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1659" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1659" s="47" t="s">
         <v>22</v>
       </c>
@@ -66464,7 +66509,10 @@
       </c>
       <c r="V1659" s="42"/>
     </row>
-    <row r="1660" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1660" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1660" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1660" s="47" t="s">
         <v>22</v>
       </c>
@@ -66493,7 +66541,10 @@
         <v>1360</v>
       </c>
     </row>
-    <row r="1661" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1661" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1661" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1661" s="47" t="s">
         <v>22</v>
       </c>
@@ -66520,7 +66571,10 @@
       </c>
       <c r="V1661" s="42"/>
     </row>
-    <row r="1662" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1662" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1662" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1662" s="47" t="s">
         <v>22</v>
       </c>
@@ -66552,7 +66606,10 @@
         <v>1362</v>
       </c>
     </row>
-    <row r="1663" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1663" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1663" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1663" s="47" t="s">
         <v>22</v>
       </c>
@@ -66581,7 +66638,10 @@
         <v>1364</v>
       </c>
     </row>
-    <row r="1664" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1664" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1664" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1664" s="47" t="s">
         <v>22</v>
       </c>
@@ -66605,7 +66665,10 @@
       </c>
       <c r="V1664" s="42"/>
     </row>
-    <row r="1665" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1665" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1665" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1665" s="47" t="s">
         <v>22</v>
       </c>
@@ -66629,7 +66692,10 @@
       </c>
       <c r="V1665" s="42"/>
     </row>
-    <row r="1666" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1666" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1666" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1666" s="47" t="s">
         <v>22</v>
       </c>
@@ -66658,7 +66724,10 @@
         <v>1367</v>
       </c>
     </row>
-    <row r="1667" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1667" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1667" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1667" s="59" t="s">
         <v>143</v>
       </c>
@@ -66690,7 +66759,10 @@
         <v>1369</v>
       </c>
     </row>
-    <row r="1668" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1668" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1668" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1668" s="59" t="s">
         <v>143</v>
       </c>
@@ -66717,7 +66789,10 @@
       </c>
       <c r="V1668" s="42"/>
     </row>
-    <row r="1669" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1669" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1669" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1669" s="59" t="s">
         <v>143</v>
       </c>
@@ -66744,7 +66819,10 @@
       </c>
       <c r="V1669" s="42"/>
     </row>
-    <row r="1670" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1670" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1670" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1670" s="59" t="s">
         <v>143</v>
       </c>
@@ -66774,7 +66852,10 @@
       </c>
       <c r="V1670" s="42"/>
     </row>
-    <row r="1671" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1671" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1671" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1671" s="59" t="s">
         <v>143</v>
       </c>
@@ -66802,7 +66883,10 @@
       <c r="U1671" s="7"/>
       <c r="V1671" s="42"/>
     </row>
-    <row r="1672" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1672" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1672" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1672" s="59" t="s">
         <v>143</v>
       </c>
@@ -66835,7 +66919,10 @@
         <v>1374</v>
       </c>
     </row>
-    <row r="1673" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1673" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1673" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1673" s="47" t="s">
         <v>22</v>
       </c>
@@ -66862,7 +66949,10 @@
       </c>
       <c r="V1673" s="42"/>
     </row>
-    <row r="1674" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1674" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1674" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1674" s="47" t="s">
         <v>22</v>
       </c>
@@ -66887,7 +66977,10 @@
       <c r="U1674" s="7"/>
       <c r="V1674" s="42"/>
     </row>
-    <row r="1675" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1675" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1675" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1675" s="47" t="s">
         <v>22</v>
       </c>
@@ -66911,7 +67004,10 @@
       </c>
       <c r="V1675" s="42"/>
     </row>
-    <row r="1676" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1676" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1676" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1676" s="47" t="s">
         <v>22</v>
       </c>
@@ -66940,7 +67036,10 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="1677" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1677" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1677" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1677" s="47" t="s">
         <v>22</v>
       </c>
@@ -66969,7 +67068,10 @@
         <v>1380</v>
       </c>
     </row>
-    <row r="1678" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1678" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1678" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1678" s="47" t="s">
         <v>22</v>
       </c>
@@ -66993,7 +67095,10 @@
       </c>
       <c r="V1678" s="42"/>
     </row>
-    <row r="1679" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1679" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1679" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1679" s="47" t="s">
         <v>22</v>
       </c>
@@ -67017,7 +67122,10 @@
       </c>
       <c r="V1679" s="42"/>
     </row>
-    <row r="1680" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1680" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1680" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1680" s="47" t="s">
         <v>22</v>
       </c>
@@ -67046,7 +67154,10 @@
         <v>1383</v>
       </c>
     </row>
-    <row r="1681" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1681" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1681" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1681" s="59" t="s">
         <v>144</v>
       </c>
@@ -67078,7 +67189,10 @@
         <v>1385</v>
       </c>
     </row>
-    <row r="1682" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1682" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1682" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1682" s="59" t="s">
         <v>144</v>
       </c>
@@ -67105,7 +67219,10 @@
       </c>
       <c r="V1682" s="42"/>
     </row>
-    <row r="1683" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1683" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1683" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1683" s="59" t="s">
         <v>144</v>
       </c>
@@ -67132,7 +67249,10 @@
       </c>
       <c r="V1683" s="42"/>
     </row>
-    <row r="1684" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1684" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1684" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1684" s="59" t="s">
         <v>144</v>
       </c>
@@ -67159,7 +67279,10 @@
       </c>
       <c r="V1684" s="42"/>
     </row>
-    <row r="1685" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1685" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1685" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1685" s="59" t="s">
         <v>144</v>
       </c>
@@ -67187,7 +67310,10 @@
       <c r="U1685" s="7"/>
       <c r="V1685" s="42"/>
     </row>
-    <row r="1686" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1686" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1686" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1686" s="47" t="s">
         <v>22</v>
       </c>
@@ -67219,7 +67345,10 @@
         <v>1390</v>
       </c>
     </row>
-    <row r="1687" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1687" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1687" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1687" s="59" t="s">
         <v>145</v>
       </c>
@@ -67246,7 +67375,10 @@
       </c>
       <c r="V1687" s="42"/>
     </row>
-    <row r="1688" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1688" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1688" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1688" s="59" t="s">
         <v>145</v>
       </c>
@@ -67273,7 +67405,10 @@
       </c>
       <c r="V1688" s="42"/>
     </row>
-    <row r="1689" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1689" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1689" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1689" s="59" t="s">
         <v>145</v>
       </c>
@@ -67300,7 +67435,10 @@
       </c>
       <c r="V1689" s="42"/>
     </row>
-    <row r="1690" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1690" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1690" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1690" s="59" t="s">
         <v>145</v>
       </c>
@@ -67333,7 +67471,10 @@
       </c>
       <c r="V1690" s="42"/>
     </row>
-    <row r="1691" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1691" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1691" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1691" s="59" t="s">
         <v>145</v>
       </c>
@@ -67365,7 +67506,10 @@
         <v>1393</v>
       </c>
     </row>
-    <row r="1692" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1692" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1692" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1692" s="47" t="s">
         <v>22</v>
       </c>
@@ -67394,7 +67538,10 @@
         <v>1395</v>
       </c>
     </row>
-    <row r="1693" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1693" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1693" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1693" s="47" t="s">
         <v>22</v>
       </c>
@@ -67418,7 +67565,10 @@
       </c>
       <c r="V1693" s="42"/>
     </row>
-    <row r="1694" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1694" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1694" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1694" s="47" t="s">
         <v>22</v>
       </c>
@@ -67442,7 +67592,10 @@
       </c>
       <c r="V1694" s="42"/>
     </row>
-    <row r="1695" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1695" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1695" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1695" s="47" t="s">
         <v>22</v>
       </c>
@@ -67466,7 +67619,10 @@
       </c>
       <c r="V1695" s="42"/>
     </row>
-    <row r="1696" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1696" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1696" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1696" s="47" t="s">
         <v>22</v>
       </c>
@@ -67495,7 +67651,10 @@
         <v>1398</v>
       </c>
     </row>
-    <row r="1697" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1697" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1697" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1697" s="47" t="s">
         <v>22</v>
       </c>
@@ -67524,7 +67683,10 @@
         <v>1400</v>
       </c>
     </row>
-    <row r="1698" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1698" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1698" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1698" s="47" t="s">
         <v>21</v>
       </c>
@@ -67552,7 +67714,10 @@
         <v>1402</v>
       </c>
     </row>
-    <row r="1699" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1699" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1699" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1699" s="59" t="s">
         <v>146</v>
       </c>
@@ -67579,7 +67744,10 @@
       </c>
       <c r="V1699" s="42"/>
     </row>
-    <row r="1700" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1700" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1700" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1700" s="59" t="s">
         <v>146</v>
       </c>
@@ -67606,7 +67774,10 @@
       </c>
       <c r="V1700" s="42"/>
     </row>
-    <row r="1701" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1701" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1701" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1701" s="59" t="s">
         <v>146</v>
       </c>
@@ -67638,7 +67809,10 @@
         <v>1405</v>
       </c>
     </row>
-    <row r="1702" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1702" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1702" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1702" s="59" t="s">
         <v>146</v>
       </c>
@@ -67665,7 +67839,10 @@
       </c>
       <c r="V1702" s="42"/>
     </row>
-    <row r="1703" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1703" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1703" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1703" s="47" t="s">
         <v>21</v>
       </c>
@@ -67689,7 +67866,10 @@
       </c>
       <c r="V1703" s="42"/>
     </row>
-    <row r="1704" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1704" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1704" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1704" s="47" t="s">
         <v>21</v>
       </c>
@@ -67713,7 +67893,10 @@
       </c>
       <c r="V1704" s="42"/>
     </row>
-    <row r="1705" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1705" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1705" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1705" s="47" t="s">
         <v>21</v>
       </c>
@@ -67742,7 +67925,10 @@
         <v>1409</v>
       </c>
     </row>
-    <row r="1706" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1706" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1706" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1706" s="47" t="s">
         <v>21</v>
       </c>
@@ -67767,7 +67953,10 @@
       <c r="U1706" s="7"/>
       <c r="V1706" s="42"/>
     </row>
-    <row r="1707" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1707" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1707" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1707" s="54" t="s">
         <v>21</v>
       </c>
@@ -67798,7 +67987,10 @@
         <v>1411</v>
       </c>
     </row>
-    <row r="1708" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1708" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1708" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1708" s="47" t="s">
         <v>21</v>
       </c>
@@ -67823,7 +68015,10 @@
       <c r="U1708" s="7"/>
       <c r="V1708" s="42"/>
     </row>
-    <row r="1709" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1709" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1709" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1709" s="47" t="s">
         <v>21</v>
       </c>
@@ -67848,7 +68043,10 @@
       <c r="U1709" s="7"/>
       <c r="V1709" s="42"/>
     </row>
-    <row r="1710" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1710" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1710" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1710" s="47" t="s">
         <v>21</v>
       </c>
@@ -67872,7 +68070,10 @@
       </c>
       <c r="V1710" s="42"/>
     </row>
-    <row r="1711" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1711" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1711" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1711" s="47" t="s">
         <v>21</v>
       </c>
@@ -67901,7 +68102,10 @@
         <v>1356</v>
       </c>
     </row>
-    <row r="1712" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1712" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1712" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1712" s="47" t="s">
         <v>21</v>
       </c>
@@ -67928,7 +68132,10 @@
       </c>
       <c r="V1712" s="42"/>
     </row>
-    <row r="1713" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1713" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1713" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1713" s="47" t="s">
         <v>21</v>
       </c>
@@ -67957,7 +68164,10 @@
         <v>1414</v>
       </c>
     </row>
-    <row r="1714" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1714" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1714" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1714" s="47" t="s">
         <v>21</v>
       </c>
@@ -67986,7 +68196,10 @@
         <v>1416</v>
       </c>
     </row>
-    <row r="1715" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1715" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1715" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1715" s="47" t="s">
         <v>21</v>
       </c>
@@ -68021,7 +68234,10 @@
         <v>1418</v>
       </c>
     </row>
-    <row r="1716" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1716" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1716" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1716" s="59" t="s">
         <v>147</v>
       </c>
@@ -68048,7 +68264,10 @@
       </c>
       <c r="V1716" s="42"/>
     </row>
-    <row r="1717" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1717" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1717" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1717" s="59" t="s">
         <v>147</v>
       </c>
@@ -68081,7 +68300,10 @@
       </c>
       <c r="V1717" s="42"/>
     </row>
-    <row r="1718" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1718" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1718" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1718" s="59" t="s">
         <v>147</v>
       </c>
@@ -68108,7 +68330,10 @@
       </c>
       <c r="V1718" s="42"/>
     </row>
-    <row r="1719" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1719" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1719" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1719" s="47" t="s">
         <v>21</v>
       </c>
@@ -68132,7 +68357,10 @@
       </c>
       <c r="V1719" s="42"/>
     </row>
-    <row r="1720" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1720" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1720" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1720" s="47" t="s">
         <v>21</v>
       </c>
@@ -68159,7 +68387,10 @@
       </c>
       <c r="V1720" s="42"/>
     </row>
-    <row r="1721" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1721" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1721" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1721" s="47" t="s">
         <v>21</v>
       </c>
@@ -68188,7 +68419,10 @@
         <v>1419</v>
       </c>
     </row>
-    <row r="1722" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1722" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1722" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1722" s="47" t="s">
         <v>21</v>
       </c>
@@ -68219,7 +68453,10 @@
       <c r="U1722" s="7"/>
       <c r="V1722" s="42"/>
     </row>
-    <row r="1723" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1723" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1723" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1723" s="47" t="s">
         <v>21</v>
       </c>
@@ -68246,7 +68483,10 @@
       <c r="U1723" s="7"/>
       <c r="V1723" s="42"/>
     </row>
-    <row r="1724" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1724" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1724" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1724" s="47" t="s">
         <v>21</v>
       </c>
@@ -68273,7 +68513,10 @@
       </c>
       <c r="V1724" s="42"/>
     </row>
-    <row r="1725" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1725" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1725" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1725" s="47" t="s">
         <v>21</v>
       </c>
@@ -68297,7 +68540,10 @@
       </c>
       <c r="V1725" s="42"/>
     </row>
-    <row r="1726" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1726" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1726" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1726" s="47" t="s">
         <v>21</v>
       </c>
@@ -68321,7 +68567,10 @@
       </c>
       <c r="V1726" s="42"/>
     </row>
-    <row r="1727" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1727" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1727" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1727" s="47" t="s">
         <v>21</v>
       </c>
@@ -68345,7 +68594,10 @@
       </c>
       <c r="V1727" s="42"/>
     </row>
-    <row r="1728" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1728" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1728" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1728" s="47" t="s">
         <v>21</v>
       </c>
@@ -68372,7 +68624,10 @@
       </c>
       <c r="V1728" s="42"/>
     </row>
-    <row r="1729" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1729" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1729" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1729" s="47" t="s">
         <v>21</v>
       </c>
@@ -68396,7 +68651,10 @@
       </c>
       <c r="V1729" s="42"/>
     </row>
-    <row r="1730" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1730" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1730" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1730" s="47" t="s">
         <v>21</v>
       </c>
@@ -68425,7 +68683,10 @@
         <v>1347</v>
       </c>
     </row>
-    <row r="1731" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1731" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1731" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1731" s="47" t="s">
         <v>21</v>
       </c>
@@ -68449,7 +68710,10 @@
       </c>
       <c r="V1731" s="42"/>
     </row>
-    <row r="1732" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1732" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1732" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1732" s="47" t="s">
         <v>21</v>
       </c>
@@ -68478,7 +68742,10 @@
         <v>1422</v>
       </c>
     </row>
-    <row r="1733" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1733" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1733" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1733" s="59" t="s">
         <v>148</v>
       </c>
@@ -68505,7 +68772,10 @@
       </c>
       <c r="V1733" s="42"/>
     </row>
-    <row r="1734" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1734" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1734" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1734" s="59" t="s">
         <v>148</v>
       </c>
@@ -68533,7 +68803,10 @@
       <c r="U1734" s="7"/>
       <c r="V1734" s="42"/>
     </row>
-    <row r="1735" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1735" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1735" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1735" s="59" t="s">
         <v>148</v>
       </c>
@@ -68563,7 +68836,10 @@
       </c>
       <c r="V1735" s="42"/>
     </row>
-    <row r="1736" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1736" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1736" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1736" s="59" t="s">
         <v>148</v>
       </c>
@@ -68598,7 +68874,10 @@
         <v>1425</v>
       </c>
     </row>
-    <row r="1737" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1737" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1737" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1737" s="47" t="s">
         <v>21</v>
       </c>
@@ -68622,7 +68901,10 @@
       </c>
       <c r="V1737" s="42"/>
     </row>
-    <row r="1738" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1738" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1738" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1738" s="47" t="s">
         <v>21</v>
       </c>
@@ -68646,7 +68928,10 @@
       </c>
       <c r="V1738" s="42"/>
     </row>
-    <row r="1739" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1739" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1739" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1739" s="47" t="s">
         <v>21</v>
       </c>
@@ -68675,7 +68960,10 @@
         <v>1428</v>
       </c>
     </row>
-    <row r="1740" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1740" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1740" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1740" s="47" t="s">
         <v>21</v>
       </c>
@@ -68707,7 +68995,10 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="1741" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1741" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1741" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1741" s="47" t="s">
         <v>21</v>
       </c>
@@ -68731,7 +69022,10 @@
       </c>
       <c r="V1741" s="42"/>
     </row>
-    <row r="1742" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1742" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1742" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1742" s="47" t="s">
         <v>21</v>
       </c>
@@ -68758,7 +69052,10 @@
       </c>
       <c r="V1742" s="42"/>
     </row>
-    <row r="1743" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1743" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1743" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1743" s="47" t="s">
         <v>21</v>
       </c>
@@ -68787,7 +69084,10 @@
         <v>1432</v>
       </c>
     </row>
-    <row r="1744" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1744" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1744" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1744" s="47" t="s">
         <v>21</v>
       </c>
@@ -68811,7 +69111,10 @@
       </c>
       <c r="V1744" s="42"/>
     </row>
-    <row r="1745" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1745" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1745" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1745" s="47" t="s">
         <v>21</v>
       </c>
@@ -68838,7 +69141,10 @@
       </c>
       <c r="V1745" s="42"/>
     </row>
-    <row r="1746" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1746" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1746" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1746" s="47" t="s">
         <v>21</v>
       </c>
@@ -68865,7 +69171,10 @@
       </c>
       <c r="V1746" s="42"/>
     </row>
-    <row r="1747" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1747" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1747" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1747" s="47" t="s">
         <v>21</v>
       </c>
@@ -68889,7 +69198,10 @@
       </c>
       <c r="V1747" s="42"/>
     </row>
-    <row r="1748" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1748" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1748" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1748" s="47" t="s">
         <v>20</v>
       </c>
@@ -68915,7 +69227,10 @@
       </c>
       <c r="V1748" s="42"/>
     </row>
-    <row r="1749" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1749" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1749" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1749" s="47" t="s">
         <v>20</v>
       </c>
@@ -68944,7 +69259,10 @@
         <v>1436</v>
       </c>
     </row>
-    <row r="1750" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1750" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1750" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1750" s="47" t="s">
         <v>20</v>
       </c>
@@ -68968,7 +69286,10 @@
       </c>
       <c r="V1750" s="42"/>
     </row>
-    <row r="1751" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1751" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1751" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1751" s="47" t="s">
         <v>20</v>
       </c>
@@ -68992,7 +69313,10 @@
       </c>
       <c r="V1751" s="42"/>
     </row>
-    <row r="1752" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1752" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1752" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1752" s="47" t="s">
         <v>20</v>
       </c>
@@ -69021,7 +69345,10 @@
         <v>1440</v>
       </c>
     </row>
-    <row r="1753" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1753" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1753" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1753" s="47" t="s">
         <v>20</v>
       </c>
@@ -69045,7 +69372,10 @@
       </c>
       <c r="V1753" s="42"/>
     </row>
-    <row r="1754" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1754" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1754" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1754" s="47" t="s">
         <v>20</v>
       </c>
@@ -69072,7 +69402,10 @@
       </c>
       <c r="V1754" s="42"/>
     </row>
-    <row r="1755" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1755" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1755" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1755" s="47" t="s">
         <v>20</v>
       </c>
@@ -69102,7 +69435,10 @@
       </c>
       <c r="V1755" s="42"/>
     </row>
-    <row r="1756" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1756" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1756" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1756" s="47" t="s">
         <v>20</v>
       </c>
@@ -69126,7 +69462,10 @@
       </c>
       <c r="V1756" s="42"/>
     </row>
-    <row r="1757" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1757" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1757" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1757" s="47" t="s">
         <v>20</v>
       </c>
@@ -69155,7 +69494,10 @@
         <v>1444</v>
       </c>
     </row>
-    <row r="1758" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1758" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1758" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1758" s="47" t="s">
         <v>20</v>
       </c>
@@ -69179,7 +69521,10 @@
       </c>
       <c r="V1758" s="42"/>
     </row>
-    <row r="1759" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1759" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1759" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1759" s="47" t="s">
         <v>20</v>
       </c>
@@ -69206,7 +69551,10 @@
       </c>
       <c r="V1759" s="42"/>
     </row>
-    <row r="1760" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1760" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1760" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1760" s="47" t="s">
         <v>20</v>
       </c>
@@ -69235,7 +69583,10 @@
         <v>1446</v>
       </c>
     </row>
-    <row r="1761" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1761" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1761" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1761" s="47" t="s">
         <v>20</v>
       </c>
@@ -69259,7 +69610,10 @@
       </c>
       <c r="V1761" s="42"/>
     </row>
-    <row r="1762" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1762" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1762" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1762" s="47" t="s">
         <v>20</v>
       </c>
@@ -69283,7 +69637,10 @@
       </c>
       <c r="V1762" s="42"/>
     </row>
-    <row r="1763" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1763" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1763" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1763" s="47" t="s">
         <v>20</v>
       </c>
@@ -69315,7 +69672,10 @@
         <v>1449</v>
       </c>
     </row>
-    <row r="1764" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1764" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1764" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1764" s="47" t="s">
         <v>20</v>
       </c>
@@ -69339,7 +69699,10 @@
       </c>
       <c r="V1764" s="42"/>
     </row>
-    <row r="1765" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1765" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1765" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1765" s="47" t="s">
         <v>20</v>
       </c>
@@ -69363,7 +69726,10 @@
       </c>
       <c r="V1765" s="42"/>
     </row>
-    <row r="1766" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1766" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1766" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1766" s="47" t="s">
         <v>20</v>
       </c>
@@ -69387,7 +69753,10 @@
       </c>
       <c r="V1766" s="42"/>
     </row>
-    <row r="1767" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1767" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1767" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1767" s="47" t="s">
         <v>20</v>
       </c>
@@ -69419,7 +69788,10 @@
         <v>1452</v>
       </c>
     </row>
-    <row r="1768" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1768" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1768" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1768" s="59" t="s">
         <v>149</v>
       </c>
@@ -69447,7 +69819,10 @@
       <c r="U1768" s="7"/>
       <c r="V1768" s="42"/>
     </row>
-    <row r="1769" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1769" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1769" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1769" s="59" t="s">
         <v>149</v>
       </c>
@@ -69475,7 +69850,10 @@
       <c r="U1769" s="7"/>
       <c r="V1769" s="42"/>
     </row>
-    <row r="1770" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1770" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1770" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1770" s="59" t="s">
         <v>149</v>
       </c>
@@ -69505,7 +69883,10 @@
       </c>
       <c r="V1770" s="42"/>
     </row>
-    <row r="1771" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1771" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1771" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1771" s="59" t="s">
         <v>149</v>
       </c>
@@ -69532,7 +69913,10 @@
       </c>
       <c r="V1771" s="42"/>
     </row>
-    <row r="1772" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1772" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1772" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1772" s="59" t="s">
         <v>149</v>
       </c>
@@ -69559,7 +69943,10 @@
       </c>
       <c r="V1772" s="42"/>
     </row>
-    <row r="1773" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1773" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1773" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1773" s="47" t="s">
         <v>20</v>
       </c>
@@ -69584,7 +69971,10 @@
       <c r="U1773" s="7"/>
       <c r="V1773" s="42"/>
     </row>
-    <row r="1774" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1774" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1774" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1774" s="47" t="s">
         <v>20</v>
       </c>
@@ -69608,7 +69998,10 @@
       </c>
       <c r="V1774" s="42"/>
     </row>
-    <row r="1775" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1775" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1775" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1775" s="47" t="s">
         <v>20</v>
       </c>
@@ -69632,7 +70025,10 @@
       </c>
       <c r="V1775" s="42"/>
     </row>
-    <row r="1776" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1776" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1776" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1776" s="47" t="s">
         <v>20</v>
       </c>
@@ -69656,7 +70052,10 @@
       </c>
       <c r="V1776" s="42"/>
     </row>
-    <row r="1777" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1777" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1777" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1777" s="47" t="s">
         <v>20</v>
       </c>
@@ -69688,7 +70087,10 @@
         <v>1456</v>
       </c>
     </row>
-    <row r="1778" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1778" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1778" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1778" s="47" t="s">
         <v>20</v>
       </c>
@@ -69712,7 +70114,10 @@
       </c>
       <c r="V1778" s="42"/>
     </row>
-    <row r="1779" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1779" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1779" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1779" s="47" t="s">
         <v>20</v>
       </c>
@@ -69736,7 +70141,10 @@
       </c>
       <c r="V1779" s="42"/>
     </row>
-    <row r="1780" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1780" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1780" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1780" s="47" t="s">
         <v>20</v>
       </c>
@@ -69760,7 +70168,10 @@
       </c>
       <c r="V1780" s="42"/>
     </row>
-    <row r="1781" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1781" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1781" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1781" s="47" t="s">
         <v>20</v>
       </c>
@@ -69784,7 +70195,10 @@
       </c>
       <c r="V1781" s="42"/>
     </row>
-    <row r="1782" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1782" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1782" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1782" s="47" t="s">
         <v>20</v>
       </c>
@@ -69808,7 +70222,10 @@
       </c>
       <c r="V1782" s="42"/>
     </row>
-    <row r="1783" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1783" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1783" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1783" s="47" t="s">
         <v>20</v>
       </c>
@@ -69832,7 +70249,10 @@
       </c>
       <c r="V1783" s="42"/>
     </row>
-    <row r="1784" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1784" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1784" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1784" s="47" t="s">
         <v>20</v>
       </c>
@@ -69856,7 +70276,10 @@
       </c>
       <c r="V1784" s="42"/>
     </row>
-    <row r="1785" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1785" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1785" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1785" s="47" t="s">
         <v>20</v>
       </c>
@@ -69888,7 +70311,10 @@
         <v>1460</v>
       </c>
     </row>
-    <row r="1786" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1786" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1786" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1786" s="47" t="s">
         <v>20</v>
       </c>
@@ -69913,7 +70339,10 @@
       <c r="U1786" s="7"/>
       <c r="V1786" s="42"/>
     </row>
-    <row r="1787" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1787" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1787" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1787" s="47" t="s">
         <v>20</v>
       </c>
@@ -69937,7 +70366,10 @@
       </c>
       <c r="V1787" s="42"/>
     </row>
-    <row r="1788" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1788" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1788" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1788" s="47" t="s">
         <v>20</v>
       </c>
@@ -69964,7 +70396,10 @@
       </c>
       <c r="V1788" s="42"/>
     </row>
-    <row r="1789" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1789" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1789" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1789" s="47" t="s">
         <v>20</v>
       </c>
@@ -69988,7 +70423,10 @@
       </c>
       <c r="V1789" s="42"/>
     </row>
-    <row r="1790" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1790" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1790" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1790" s="47" t="s">
         <v>20</v>
       </c>
@@ -70012,7 +70450,10 @@
       </c>
       <c r="V1790" s="42"/>
     </row>
-    <row r="1791" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1791" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1791" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1791" s="47" t="s">
         <v>20</v>
       </c>
@@ -70041,7 +70482,10 @@
         <v>1465</v>
       </c>
     </row>
-    <row r="1792" spans="9:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1792" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1792" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1792" s="47" t="s">
         <v>20</v>
       </c>
@@ -70070,7 +70514,10 @@
         <v>1467</v>
       </c>
     </row>
-    <row r="1793" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1793" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1793" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1793" s="47" t="s">
         <v>20</v>
       </c>
@@ -70099,7 +70546,10 @@
         <v>1469</v>
       </c>
     </row>
-    <row r="1794" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1794" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1794" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1794" s="47" t="s">
         <v>20</v>
       </c>
@@ -70131,7 +70581,10 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="1795" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1795" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1795" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1795" s="47" t="s">
         <v>20</v>
       </c>
@@ -70155,7 +70608,10 @@
       </c>
       <c r="V1795" s="42"/>
     </row>
-    <row r="1796" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1796" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1796" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1796" s="47" t="s">
         <v>20</v>
       </c>
@@ -70179,7 +70635,10 @@
       </c>
       <c r="V1796" s="42"/>
     </row>
-    <row r="1797" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1797" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1797" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1797" s="47" t="s">
         <v>20</v>
       </c>
@@ -70206,7 +70665,10 @@
       </c>
       <c r="V1797" s="42"/>
     </row>
-    <row r="1798" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1798" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1798" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1798" s="47" t="s">
         <v>20</v>
       </c>
@@ -70233,7 +70695,10 @@
       </c>
       <c r="V1798" s="42"/>
     </row>
-    <row r="1799" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1799" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1799" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1799" s="47" t="s">
         <v>20</v>
       </c>
@@ -70257,7 +70722,10 @@
       </c>
       <c r="V1799" s="42"/>
     </row>
-    <row r="1800" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1800" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1800" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1800" s="47" t="s">
         <v>20</v>
       </c>
@@ -70281,7 +70749,10 @@
       </c>
       <c r="V1800" s="42"/>
     </row>
-    <row r="1801" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1801" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1801" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1801" s="47" t="s">
         <v>20</v>
       </c>
@@ -70305,7 +70776,10 @@
       </c>
       <c r="V1801" s="42"/>
     </row>
-    <row r="1802" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1802" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1802" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1802" s="47" t="s">
         <v>20</v>
       </c>
@@ -70334,7 +70808,10 @@
         <v>1476</v>
       </c>
     </row>
-    <row r="1803" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1803" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1803" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1803" s="47" t="s">
         <v>20</v>
       </c>
@@ -70358,7 +70835,10 @@
       </c>
       <c r="V1803" s="42"/>
     </row>
-    <row r="1804" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1804" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1804" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1804" s="47" t="s">
         <v>20</v>
       </c>
@@ -70382,7 +70862,10 @@
       </c>
       <c r="V1804" s="42"/>
     </row>
-    <row r="1805" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1805" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1805" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="I1805" s="47" t="s">
         <v>20</v>
       </c>
@@ -70414,7 +70897,10 @@
         <v>1480</v>
       </c>
     </row>
-    <row r="1806" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1806" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1806" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1806" s="59" t="s">
         <v>150</v>
       </c>
@@ -70441,7 +70927,10 @@
       </c>
       <c r="V1806" s="42"/>
     </row>
-    <row r="1807" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1807" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1807" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1807" s="59" t="s">
         <v>150</v>
       </c>
@@ -70471,7 +70960,10 @@
       </c>
       <c r="V1807" s="42"/>
     </row>
-    <row r="1808" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1808" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1808" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1808" s="59" t="s">
         <v>150</v>
       </c>
@@ -70498,7 +70990,10 @@
       </c>
       <c r="V1808" s="42"/>
     </row>
-    <row r="1809" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1809" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1809" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1809" s="59" t="s">
         <v>150</v>
       </c>
@@ -70525,7 +71020,10 @@
       </c>
       <c r="V1809" s="42"/>
     </row>
-    <row r="1810" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1810" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1810" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1810" s="59" t="s">
         <v>150</v>
       </c>
@@ -70555,7 +71053,10 @@
       </c>
       <c r="V1810" s="42"/>
     </row>
-    <row r="1811" spans="8:22" ht="20.25" x14ac:dyDescent="0.25">
+    <row r="1811" spans="3:22" ht="20.25" x14ac:dyDescent="0.25">
+      <c r="C1811" s="63" t="s">
+        <v>1487</v>
+      </c>
       <c r="H1811" s="59" t="s">
         <v>150</v>
       </c>
@@ -70587,7 +71088,7 @@
         <v>1483</v>
       </c>
     </row>
-    <row r="1812" spans="8:22" x14ac:dyDescent="0.25">
+    <row r="1812" spans="3:22" x14ac:dyDescent="0.25">
       <c r="P1812" s="7"/>
     </row>
   </sheetData>

</xml_diff>